<commit_message>
initial climbview support in makemuzicodes
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine2.xlsx
+++ b/scoretools/test/mkGameEngine2.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="380" windowWidth="25040" windowHeight="15500"/>
+    <workbookView xWindow="1020" yWindow="375" windowWidth="25035" windowHeight="15495"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
   <si>
     <t>stage</t>
   </si>
@@ -75,9 +80,6 @@
     <t>monitor</t>
   </si>
   <si>
-    <t>visual</t>
-  </si>
-  <si>
     <t>mc2:</t>
   </si>
   <si>
@@ -160,6 +162,15 @@
   </si>
   <si>
     <t>91147f</t>
+  </si>
+  <si>
+    <t>v.background</t>
+  </si>
+  <si>
+    <t>v.animate</t>
+  </si>
+  <si>
+    <t>v.mc</t>
   </si>
 </sst>
 </file>
@@ -498,7 +509,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,37 +517,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC5"/>
+  <dimension ref="A1:AE5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" customWidth="1"/>
-    <col min="2" max="2" width="30.33203125" customWidth="1"/>
-    <col min="3" max="8" width="5.6640625" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" customWidth="1"/>
-    <col min="10" max="10" width="5.1640625" customWidth="1"/>
-    <col min="11" max="12" width="9.1640625" customWidth="1"/>
-    <col min="13" max="14" width="12.1640625" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" customWidth="1"/>
+    <col min="3" max="8" width="5.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.140625" customWidth="1"/>
+    <col min="10" max="10" width="5.140625" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" customWidth="1"/>
+    <col min="13" max="14" width="12.140625" customWidth="1"/>
     <col min="15" max="15" width="5" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" customWidth="1"/>
-    <col min="17" max="17" width="6.5" customWidth="1"/>
-    <col min="18" max="18" width="10.33203125" customWidth="1"/>
-    <col min="19" max="19" width="6.5" customWidth="1"/>
-    <col min="20" max="20" width="5.1640625" customWidth="1"/>
-    <col min="21" max="21" width="22.5" customWidth="1"/>
-    <col min="22" max="22" width="5.6640625" customWidth="1"/>
-    <col min="23" max="23" width="6.83203125" customWidth="1"/>
-    <col min="25" max="25" width="23.6640625" customWidth="1"/>
-    <col min="26" max="26" width="20.1640625" customWidth="1"/>
-    <col min="27" max="27" width="6.5" customWidth="1"/>
-    <col min="28" max="28" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="19.7109375" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" customWidth="1"/>
+    <col min="18" max="20" width="10.28515625" customWidth="1"/>
+    <col min="21" max="21" width="6.42578125" customWidth="1"/>
+    <col min="22" max="22" width="5.140625" customWidth="1"/>
+    <col min="23" max="23" width="22.42578125" customWidth="1"/>
+    <col min="24" max="24" width="5.7109375" customWidth="1"/>
+    <col min="25" max="25" width="6.85546875" customWidth="1"/>
+    <col min="27" max="27" width="23.7109375" customWidth="1"/>
+    <col min="28" max="28" width="20.140625" customWidth="1"/>
+    <col min="29" max="29" width="6.42578125" customWidth="1"/>
+    <col min="30" max="30" width="6.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="1" customFormat="1">
+    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -544,7 +555,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>8</v>
@@ -571,66 +582,72 @@
         <v>15</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>17</v>
+        <v>45</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="W1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="X1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="AA1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="AB1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="AE1" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:29">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -657,39 +674,39 @@
         <v>4</v>
       </c>
       <c r="N2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" t="s">
+        <v>26</v>
+      </c>
+      <c r="W2" t="s">
         <v>27</v>
       </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
+        <v>4</v>
+      </c>
+      <c r="Z2" t="s">
         <v>28</v>
       </c>
-      <c r="V2" t="s">
-        <v>4</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="AB2" t="s">
         <v>29</v>
       </c>
-      <c r="Z2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AC2" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" t="s">
-        <v>45</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>32</v>
+      <c r="AD2" t="s">
+        <v>44</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:29">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
         <v>3</v>
@@ -716,27 +733,30 @@
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="Q3" t="s">
         <v>5</v>
       </c>
-      <c r="S3" t="s">
-        <v>35</v>
+      <c r="T3">
+        <v>1</v>
+      </c>
+      <c r="U3" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:29">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
@@ -757,18 +777,18 @@
         <v>3</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="P4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:29">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>3</v>
@@ -789,19 +809,22 @@
         <v>3</v>
       </c>
       <c r="L5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N5" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" t="s">
         <v>43</v>
       </c>
-      <c r="P5" t="s">
-        <v>44</v>
-      </c>
       <c r="R5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="S5" t="s">
-        <v>36</v>
+        <v>35</v>
+      </c>
+      <c r="U5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
support for delay to v.mc and midi2; single trigger of code per stage
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine2.xlsx
+++ b/scoretools/test/mkGameEngine2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="27430"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="114">
   <si>
     <t>stage</t>
   </si>
@@ -349,6 +349,21 @@
   </si>
   <si>
     <t>v.mc</t>
+  </si>
+  <si>
+    <t>delay</t>
+  </si>
+  <si>
+    <t>next</t>
+  </si>
+  <si>
+    <t>end</t>
+  </si>
+  <si>
+    <t>midi2</t>
+  </si>
+  <si>
+    <t>anim.jpg</t>
   </si>
 </sst>
 </file>
@@ -496,8 +511,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="183">
+  <cellStyleXfs count="197">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -709,7 +738,7 @@
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
-  <cellStyles count="183">
+  <cellStyles count="197">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -801,6 +830,13 @@
     <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -892,6 +928,13 @@
     <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1162,7 +1205,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1170,191 +1213,202 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO19"/>
+  <dimension ref="A1:AR19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" workbookViewId="0">
-      <selection activeCell="U5" sqref="U5"/>
+    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="Z4" sqref="Z4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="12.1640625" style="14" customWidth="1"/>
-    <col min="2" max="2" width="32.1640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="7.6640625" style="11" customWidth="1"/>
-    <col min="4" max="4" width="9.1640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="8.83203125" style="11" customWidth="1"/>
-    <col min="6" max="6" width="9.1640625" style="11" customWidth="1"/>
-    <col min="7" max="7" width="8.33203125" style="11" customWidth="1"/>
-    <col min="8" max="8" width="9.1640625" style="11" customWidth="1"/>
-    <col min="9" max="9" width="12.1640625" style="16" customWidth="1"/>
-    <col min="10" max="10" width="9.33203125" style="16" customWidth="1"/>
-    <col min="11" max="12" width="9.83203125" style="16" customWidth="1"/>
-    <col min="13" max="14" width="12.1640625" style="16" customWidth="1"/>
-    <col min="15" max="15" width="23.1640625" style="7" customWidth="1"/>
-    <col min="16" max="16" width="19.6640625" style="7" customWidth="1"/>
-    <col min="17" max="17" width="6.5" style="7" customWidth="1"/>
-    <col min="18" max="18" width="9.6640625" style="7" customWidth="1"/>
-    <col min="19" max="19" width="14" style="7" customWidth="1"/>
-    <col min="20" max="21" width="11.6640625" style="7" customWidth="1"/>
-    <col min="22" max="22" width="24" style="3" customWidth="1"/>
-    <col min="23" max="23" width="17.83203125" style="3" customWidth="1"/>
-    <col min="24" max="24" width="5.6640625" style="3" customWidth="1"/>
-    <col min="25" max="25" width="6.83203125" style="3" customWidth="1"/>
-    <col min="26" max="26" width="8.83203125" style="3"/>
-    <col min="27" max="27" width="19.33203125" style="5" customWidth="1"/>
-    <col min="28" max="28" width="20.1640625" style="5" customWidth="1"/>
-    <col min="29" max="29" width="6.5" style="5" customWidth="1"/>
-    <col min="30" max="30" width="6.6640625" style="5" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="5"/>
-    <col min="32" max="32" width="22.83203125" style="11" customWidth="1"/>
-    <col min="33" max="33" width="20.1640625" style="11" customWidth="1"/>
-    <col min="34" max="34" width="6.5" style="11" customWidth="1"/>
-    <col min="35" max="35" width="6.6640625" style="11" customWidth="1"/>
-    <col min="36" max="36" width="8.83203125" style="11"/>
-    <col min="37" max="37" width="20.6640625" style="11" customWidth="1"/>
-    <col min="38" max="38" width="20.1640625" style="11" customWidth="1"/>
-    <col min="39" max="39" width="6.5" style="11" customWidth="1"/>
-    <col min="40" max="40" width="6.6640625" style="11" customWidth="1"/>
-    <col min="41" max="41" width="8.83203125" style="11"/>
+    <col min="1" max="2" width="12.1640625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" style="10" customWidth="1"/>
+    <col min="4" max="4" width="7.6640625" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9.1640625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.1640625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.1640625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="12.1640625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="9.33203125" style="16" customWidth="1"/>
+    <col min="12" max="13" width="9.83203125" style="16" customWidth="1"/>
+    <col min="14" max="15" width="12.1640625" style="16" customWidth="1"/>
+    <col min="16" max="16" width="23.1640625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" style="7" customWidth="1"/>
+    <col min="18" max="18" width="6.5" style="7" customWidth="1"/>
+    <col min="19" max="19" width="9.6640625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="14" style="7" customWidth="1"/>
+    <col min="21" max="21" width="11.6640625" style="7" customWidth="1"/>
+    <col min="22" max="22" width="6.1640625" style="7" customWidth="1"/>
+    <col min="23" max="24" width="11.6640625" style="7" customWidth="1"/>
+    <col min="25" max="25" width="24" style="3" customWidth="1"/>
+    <col min="26" max="26" width="17.83203125" style="3" customWidth="1"/>
+    <col min="27" max="27" width="5.6640625" style="3" customWidth="1"/>
+    <col min="28" max="28" width="6.83203125" style="3" customWidth="1"/>
+    <col min="29" max="29" width="8.83203125" style="3"/>
+    <col min="30" max="30" width="19.33203125" style="5" customWidth="1"/>
+    <col min="31" max="31" width="20.1640625" style="5" customWidth="1"/>
+    <col min="32" max="32" width="6.5" style="5" customWidth="1"/>
+    <col min="33" max="33" width="6.6640625" style="5" customWidth="1"/>
+    <col min="34" max="34" width="8.83203125" style="5"/>
+    <col min="35" max="35" width="22.83203125" style="11" customWidth="1"/>
+    <col min="36" max="36" width="20.1640625" style="11" customWidth="1"/>
+    <col min="37" max="37" width="6.5" style="11" customWidth="1"/>
+    <col min="38" max="38" width="6.6640625" style="11" customWidth="1"/>
+    <col min="39" max="39" width="8.83203125" style="11"/>
+    <col min="40" max="40" width="20.6640625" style="11" customWidth="1"/>
+    <col min="41" max="41" width="20.1640625" style="11" customWidth="1"/>
+    <col min="42" max="42" width="6.5" style="11" customWidth="1"/>
+    <col min="43" max="43" width="6.6640625" style="11" customWidth="1"/>
+    <col min="44" max="44" width="8.83203125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="1" customFormat="1">
+    <row r="1" spans="1:44" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="D1" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="D1" s="9" t="s">
+      <c r="E1" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="F1" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="G1" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="9" t="s">
+      <c r="H1" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="I1" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="15" t="s">
+      <c r="J1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="J1" s="15" t="s">
+      <c r="K1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="15" t="s">
+      <c r="L1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="L1" s="15" t="s">
+      <c r="M1" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="N1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>106</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="S1" s="6" t="s">
+      <c r="T1" s="6" t="s">
         <v>15</v>
-      </c>
-      <c r="T1" s="6" t="s">
-        <v>107</v>
       </c>
       <c r="U1" s="6" t="s">
         <v>108</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="W1" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="X1" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AA1" s="4" t="s">
+      <c r="AD1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="9" t="s">
+      <c r="AI1" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="AG1" s="9" t="s">
+      <c r="AJ1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AH1" s="9" t="s">
+      <c r="AK1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AI1" s="9" t="s">
+      <c r="AL1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AJ1" s="9" t="s">
+      <c r="AM1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AK1" s="9" t="s">
+      <c r="AN1" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="AL1" s="9" t="s">
+      <c r="AO1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AM1" s="9" t="s">
+      <c r="AP1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AN1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:41">
+    <row r="2" spans="1:44">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D2" s="11" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="E2" s="11" t="s">
         <v>3</v>
@@ -1368,64 +1422,76 @@
       <c r="H2" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="I2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="7" t="s">
+      <c r="P2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="P2" s="7" t="s">
+      <c r="Q2" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="R2" s="7" t="s">
+      <c r="S2" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="V2" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="X2" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="11" t="s">
+      <c r="AC2" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="AJ2" s="5"/>
-      <c r="AO2" s="5"/>
+      <c r="AM2" s="5"/>
+      <c r="AR2" s="5"/>
     </row>
-    <row r="3" spans="1:41">
+    <row r="3" spans="1:44">
       <c r="A3" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D3" s="11" t="s">
         <v>5</v>
       </c>
@@ -1441,42 +1507,45 @@
       <c r="H3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="7" t="s">
+      <c r="I3" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P3" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="P3" s="7" t="s">
+      <c r="Q3" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="R3" s="18" t="s">
+      <c r="S3" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="V3" s="3" t="s">
+      <c r="Y3" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="W3" s="7" t="s">
+      <c r="Z3" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="X3" s="3" t="s">
+      <c r="AA3" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Y3" s="3" t="s">
+      <c r="AB3" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:41">
+    <row r="4" spans="1:44">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="C4" s="11" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="12" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="11" t="s">
+      <c r="D4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="12" t="s">
         <v>3</v>
       </c>
       <c r="F4" s="11" t="s">
@@ -1488,35 +1557,41 @@
       <c r="H4" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="I4" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L4" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O4" s="7" t="s">
+      <c r="P4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="7" t="s">
+      <c r="Q4" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="Q4" s="7" t="s">
+      <c r="R4" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="R4" s="7" t="s">
+      <c r="S4" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="S4" s="7" t="s">
+      <c r="T4" s="7" t="s">
         <v>24</v>
       </c>
+      <c r="Z4" s="7" t="s">
+        <v>80</v>
+      </c>
     </row>
-    <row r="5" spans="1:41">
+    <row r="5" spans="1:44">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="B5" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="C5" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D5" s="11" t="s">
         <v>3</v>
       </c>
@@ -1532,40 +1607,43 @@
       <c r="H5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="N5" s="7"/>
-      <c r="O5" s="7" t="s">
+      <c r="I5" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="P5" s="7" t="s">
+      <c r="Q5" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="R5" s="18" t="s">
+      <c r="S5" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="V5" s="7" t="s">
+      <c r="Y5" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="W5" s="7" t="s">
+      <c r="Z5" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="X5" s="7" t="s">
+      <c r="AA5" s="7" t="s">
         <v>82</v>
       </c>
-      <c r="Y5" s="18" t="s">
+      <c r="AB5" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="Z5" s="7"/>
+      <c r="AC5" s="7"/>
     </row>
-    <row r="6" spans="1:41">
+    <row r="6" spans="1:44">
       <c r="A6" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="14" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="C6" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D6" s="11" t="s">
         <v>5</v>
       </c>
@@ -1581,23 +1659,24 @@
       <c r="H6" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K6" s="16" t="s">
+      <c r="I6" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="O6" s="7" t="s">
+      <c r="P6" s="7" t="s">
         <v>94</v>
       </c>
-      <c r="P6" s="17" t="s">
+      <c r="Q6" s="17" t="s">
         <v>83</v>
       </c>
-      <c r="Q6" s="17"/>
-      <c r="R6" s="17" t="s">
+      <c r="R6" s="17"/>
+      <c r="S6" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="S6" s="17"/>
       <c r="T6" s="17"/>
       <c r="U6" s="17"/>
-      <c r="V6" s="17"/>
       <c r="W6" s="17"/>
       <c r="X6" s="17"/>
       <c r="Y6" s="17"/>
@@ -1617,19 +1696,22 @@
       <c r="AM6" s="17"/>
       <c r="AN6" s="17"/>
       <c r="AO6" s="17"/>
+      <c r="AP6" s="17"/>
+      <c r="AQ6" s="17"/>
+      <c r="AR6" s="17"/>
     </row>
-    <row r="7" spans="1:41">
+    <row r="7" spans="1:44">
       <c r="A7" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="B7" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C7" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D7" s="11" t="s">
-        <v>70</v>
+        <v>5</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>70</v>
@@ -1643,10 +1725,12 @@
       <c r="H7" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="16" t="s">
+      <c r="I7" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="M7" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="O7" s="17"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="17"/>
       <c r="R7" s="17"/>
@@ -1673,17 +1757,20 @@
       <c r="AM7" s="17"/>
       <c r="AN7" s="17"/>
       <c r="AO7" s="17"/>
+      <c r="AP7" s="17"/>
+      <c r="AQ7" s="17"/>
+      <c r="AR7" s="17"/>
     </row>
-    <row r="8" spans="1:41">
+    <row r="8" spans="1:44">
       <c r="A8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="C8" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D8" s="11" t="s">
         <v>3</v>
       </c>
@@ -1699,33 +1786,36 @@
       <c r="H8" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="16" t="s">
+      <c r="I8" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="O8" s="7" t="s">
+      <c r="P8" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="P8" s="7" t="s">
+      <c r="Q8" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="Q8" s="7" t="s">
+      <c r="R8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="R8" s="7" t="s">
+      <c r="S8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="W8" s="17"/>
+      <c r="Z8" s="17"/>
     </row>
-    <row r="9" spans="1:41">
+    <row r="9" spans="1:44">
       <c r="A9" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="C9" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D9" s="11" t="s">
         <v>5</v>
       </c>
@@ -1741,13 +1831,15 @@
       <c r="H9" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="I9" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="O9" s="17"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="17"/>
       <c r="R9" s="17"/>
@@ -1774,17 +1866,20 @@
       <c r="AM9" s="17"/>
       <c r="AN9" s="17"/>
       <c r="AO9" s="17"/>
+      <c r="AP9" s="17"/>
+      <c r="AQ9" s="17"/>
+      <c r="AR9" s="17"/>
     </row>
-    <row r="10" spans="1:41">
+    <row r="10" spans="1:44">
       <c r="A10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D10" s="11" t="s">
         <v>5</v>
       </c>
@@ -1800,10 +1895,12 @@
       <c r="H10" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="I10" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="M10" s="16" t="s">
         <v>73</v>
       </c>
-      <c r="O10" s="17"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="17"/>
       <c r="R10" s="17"/>
@@ -1830,17 +1927,20 @@
       <c r="AM10" s="17"/>
       <c r="AN10" s="17"/>
       <c r="AO10" s="17"/>
+      <c r="AP10" s="17"/>
+      <c r="AQ10" s="17"/>
+      <c r="AR10" s="17"/>
     </row>
-    <row r="11" spans="1:41">
+    <row r="11" spans="1:44">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="B11" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C11" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D11" s="11" t="s">
         <v>5</v>
       </c>
@@ -1856,13 +1956,15 @@
       <c r="H11" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="I11" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L11" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="O11" s="17"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="17"/>
       <c r="R11" s="17"/>
@@ -1889,17 +1991,20 @@
       <c r="AM11" s="17"/>
       <c r="AN11" s="17"/>
       <c r="AO11" s="17"/>
+      <c r="AP11" s="17"/>
+      <c r="AQ11" s="17"/>
+      <c r="AR11" s="17"/>
     </row>
-    <row r="12" spans="1:41" ht="13" customHeight="1">
+    <row r="12" spans="1:44" ht="13" customHeight="1">
       <c r="A12" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="C12" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D12" s="11" t="s">
         <v>5</v>
       </c>
@@ -1915,13 +2020,15 @@
       <c r="H12" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="K12" s="16" t="s">
+      <c r="I12" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="L12" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="L12" s="16" t="s">
+      <c r="M12" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="O12" s="17"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="17"/>
       <c r="R12" s="17"/>
@@ -1948,17 +2055,20 @@
       <c r="AM12" s="17"/>
       <c r="AN12" s="17"/>
       <c r="AO12" s="17"/>
+      <c r="AP12" s="17"/>
+      <c r="AQ12" s="17"/>
+      <c r="AR12" s="17"/>
     </row>
-    <row r="13" spans="1:41">
+    <row r="13" spans="1:44">
       <c r="A13" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="B13" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="11" t="s">
-        <v>3</v>
-      </c>
       <c r="D13" s="11" t="s">
         <v>3</v>
       </c>
@@ -1974,10 +2084,12 @@
       <c r="H13" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="I13" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="M13" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="O13" s="17"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
@@ -2004,17 +2116,20 @@
       <c r="AM13" s="17"/>
       <c r="AN13" s="17"/>
       <c r="AO13" s="17"/>
+      <c r="AP13" s="17"/>
+      <c r="AQ13" s="17"/>
+      <c r="AR13" s="17"/>
     </row>
-    <row r="14" spans="1:41">
+    <row r="14" spans="1:44">
       <c r="A14" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="C14" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="C14" s="11" t="s">
-        <v>5</v>
-      </c>
       <c r="D14" s="11" t="s">
         <v>5</v>
       </c>
@@ -2030,60 +2145,65 @@
       <c r="H14" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="I14" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="P14" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="P14" s="7" t="s">
+      <c r="Q14" s="7" t="s">
         <v>85</v>
       </c>
-      <c r="R14" s="7" t="s">
+      <c r="S14" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="V14" s="7" t="s">
+      <c r="Y14" s="7" t="s">
         <v>96</v>
       </c>
-      <c r="W14" s="7" t="s">
+      <c r="Z14" s="7" t="s">
         <v>86</v>
       </c>
-      <c r="Y14" s="3" t="s">
+      <c r="AB14" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AA14" s="7" t="s">
+      <c r="AD14" s="7" t="s">
         <v>97</v>
       </c>
-      <c r="AB14" s="19" t="s">
+      <c r="AE14" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="AD14" s="5" t="s">
+      <c r="AG14" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="AF14" s="11" t="s">
+      <c r="AI14" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AG14" s="20" t="s">
+      <c r="AJ14" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="AI14" s="11" t="s">
+      <c r="AL14" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="AK14" s="11" t="s">
+      <c r="AN14" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="AL14" s="20" t="s">
+      <c r="AO14" s="20" t="s">
         <v>91</v>
       </c>
-      <c r="AN14" s="11" t="s">
+      <c r="AQ14" s="11" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="15" spans="1:41">
+    <row r="15" spans="1:44">
       <c r="A15" s="14" t="s">
         <v>102</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="O15" s="17"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="17"/>
       <c r="R15" s="17"/>
@@ -2110,15 +2230,20 @@
       <c r="AM15" s="17"/>
       <c r="AN15" s="17"/>
       <c r="AO15" s="17"/>
+      <c r="AP15" s="17"/>
+      <c r="AQ15" s="17"/>
+      <c r="AR15" s="17"/>
     </row>
-    <row r="16" spans="1:41">
+    <row r="16" spans="1:44">
       <c r="A16" s="21" t="s">
         <v>103</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="B16" s="21" t="s">
+        <v>111</v>
+      </c>
+      <c r="C16" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="O16" s="17"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="17"/>
       <c r="R16" s="17"/>
@@ -2145,9 +2270,16 @@
       <c r="AM16" s="17"/>
       <c r="AN16" s="17"/>
       <c r="AO16" s="17"/>
+      <c r="AP16" s="17"/>
+      <c r="AQ16" s="17"/>
+      <c r="AR16" s="17"/>
     </row>
-    <row r="19" spans="15:41">
-      <c r="O19" s="17"/>
+    <row r="17" spans="1:44">
+      <c r="A17" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:44">
       <c r="P19" s="17"/>
       <c r="Q19" s="17"/>
       <c r="R19" s="17"/>
@@ -2174,10 +2306,13 @@
       <c r="AM19" s="17"/>
       <c r="AN19" s="17"/>
       <c r="AO19" s="17"/>
+      <c r="AP19" s="17"/>
+      <c r="AQ19" s="17"/>
+      <c r="AR19" s="17"/>
     </row>
   </sheetData>
-  <sortState ref="X5:Z6">
-    <sortCondition descending="1" ref="Z5"/>
+  <sortState ref="AA5:AC6">
+    <sortCondition descending="1" ref="AC5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
added v.mc.delay option to experience generator
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine2.xlsx
+++ b/scoretools/test/mkGameEngine2.xlsx
@@ -1,28 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="26330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pszcmg\workspace\fast-performance-demo\scoretools\test\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="13920"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25365" windowHeight="13920"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="150">
   <si>
     <t>stage</t>
   </si>
@@ -469,13 +474,16 @@
   </si>
   <si>
     <t>4bAHallucination.mei</t>
+  </si>
+  <si>
+    <t>v.mc.delay</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1538,7 +1546,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1546,64 +1554,64 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB68"/>
+  <dimension ref="A1:BC68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+      <selection activeCell="AP2" sqref="AP2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="12.1640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="29.5" style="10" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" style="11" customWidth="1"/>
-    <col min="5" max="5" width="9.1640625" style="11" customWidth="1"/>
-    <col min="6" max="6" width="8.83203125" style="11" customWidth="1"/>
-    <col min="7" max="7" width="9.1640625" style="11" customWidth="1"/>
-    <col min="8" max="8" width="8.33203125" style="11" customWidth="1"/>
-    <col min="9" max="9" width="9.1640625" style="11" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" style="16" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" style="16" customWidth="1"/>
-    <col min="12" max="13" width="9.83203125" style="16" customWidth="1"/>
-    <col min="14" max="14" width="5.83203125" style="16" customWidth="1"/>
-    <col min="15" max="15" width="9.83203125" style="16" customWidth="1"/>
+    <col min="1" max="2" width="12.140625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="29.42578125" style="10" customWidth="1"/>
+    <col min="4" max="4" width="7.7109375" style="11" customWidth="1"/>
+    <col min="5" max="5" width="9.140625" style="11" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="11" customWidth="1"/>
+    <col min="8" max="8" width="8.28515625" style="11" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="11" customWidth="1"/>
+    <col min="10" max="10" width="12.140625" style="16" customWidth="1"/>
+    <col min="11" max="11" width="9.28515625" style="16" customWidth="1"/>
+    <col min="12" max="13" width="9.85546875" style="16" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" style="16" customWidth="1"/>
+    <col min="15" max="15" width="9.85546875" style="16" customWidth="1"/>
     <col min="16" max="16" width="8" style="16" customWidth="1"/>
-    <col min="17" max="17" width="12.1640625" style="16" customWidth="1"/>
-    <col min="18" max="18" width="12.5" style="16" customWidth="1"/>
-    <col min="19" max="19" width="5.6640625" style="16" customWidth="1"/>
-    <col min="20" max="20" width="23.1640625" style="7" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" style="7" customWidth="1"/>
-    <col min="22" max="22" width="7.6640625" style="7" customWidth="1"/>
+    <col min="17" max="17" width="12.140625" style="16" customWidth="1"/>
+    <col min="18" max="18" width="12.42578125" style="16" customWidth="1"/>
+    <col min="19" max="19" width="5.7109375" style="16" customWidth="1"/>
+    <col min="20" max="20" width="23.140625" style="7" customWidth="1"/>
+    <col min="21" max="21" width="10.85546875" style="7" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" style="7" customWidth="1"/>
     <col min="23" max="23" width="7" style="7" customWidth="1"/>
-    <col min="24" max="24" width="8.33203125" style="7" customWidth="1"/>
-    <col min="25" max="25" width="9.5" style="7" customWidth="1"/>
-    <col min="26" max="26" width="12.1640625" style="7" customWidth="1"/>
-    <col min="27" max="27" width="24" style="3" customWidth="1"/>
-    <col min="28" max="28" width="11.1640625" style="3" customWidth="1"/>
-    <col min="29" max="29" width="8.33203125" style="3" customWidth="1"/>
-    <col min="30" max="30" width="6.83203125" style="3" customWidth="1"/>
-    <col min="31" max="31" width="8.83203125" style="3"/>
-    <col min="32" max="32" width="14.6640625" style="3" customWidth="1"/>
-    <col min="33" max="33" width="9.33203125" style="3" customWidth="1"/>
-    <col min="34" max="34" width="19.33203125" style="5" customWidth="1"/>
-    <col min="35" max="35" width="11" style="5" customWidth="1"/>
-    <col min="36" max="36" width="6.83203125" style="5" customWidth="1"/>
-    <col min="37" max="37" width="6.6640625" style="5" customWidth="1"/>
-    <col min="38" max="40" width="8.83203125" style="5"/>
-    <col min="41" max="41" width="13" style="11" customWidth="1"/>
-    <col min="42" max="42" width="20.1640625" style="11" customWidth="1"/>
-    <col min="43" max="43" width="6.5" style="11" customWidth="1"/>
-    <col min="44" max="44" width="6.6640625" style="11" customWidth="1"/>
-    <col min="45" max="47" width="8.83203125" style="11"/>
-    <col min="48" max="48" width="20.6640625" style="11" customWidth="1"/>
-    <col min="49" max="49" width="20.1640625" style="11" customWidth="1"/>
-    <col min="50" max="50" width="6.5" style="11" customWidth="1"/>
-    <col min="51" max="51" width="6.6640625" style="11" customWidth="1"/>
-    <col min="52" max="52" width="8.83203125" style="11"/>
-    <col min="53" max="54" width="8.83203125" style="30"/>
+    <col min="24" max="24" width="8.28515625" style="7" customWidth="1"/>
+    <col min="25" max="26" width="9.42578125" style="7" customWidth="1"/>
+    <col min="27" max="27" width="12.140625" style="7" customWidth="1"/>
+    <col min="28" max="28" width="24" style="3" customWidth="1"/>
+    <col min="29" max="29" width="11.140625" style="3" customWidth="1"/>
+    <col min="30" max="30" width="8.28515625" style="3" customWidth="1"/>
+    <col min="31" max="31" width="6.85546875" style="3" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" style="3"/>
+    <col min="33" max="33" width="14.7109375" style="3" customWidth="1"/>
+    <col min="34" max="34" width="9.28515625" style="3" customWidth="1"/>
+    <col min="35" max="35" width="19.28515625" style="5" customWidth="1"/>
+    <col min="36" max="36" width="11" style="5" customWidth="1"/>
+    <col min="37" max="37" width="6.85546875" style="5" customWidth="1"/>
+    <col min="38" max="38" width="6.7109375" style="5" customWidth="1"/>
+    <col min="39" max="41" width="8.85546875" style="5"/>
+    <col min="42" max="42" width="13" style="11" customWidth="1"/>
+    <col min="43" max="43" width="20.140625" style="11" customWidth="1"/>
+    <col min="44" max="44" width="6.42578125" style="11" customWidth="1"/>
+    <col min="45" max="45" width="6.7109375" style="11" customWidth="1"/>
+    <col min="46" max="48" width="8.85546875" style="11"/>
+    <col min="49" max="49" width="20.7109375" style="11" customWidth="1"/>
+    <col min="50" max="50" width="20.140625" style="11" customWidth="1"/>
+    <col min="51" max="51" width="6.42578125" style="11" customWidth="1"/>
+    <col min="52" max="52" width="6.7109375" style="11" customWidth="1"/>
+    <col min="53" max="53" width="8.85546875" style="11"/>
+    <col min="54" max="55" width="8.85546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" s="1" customFormat="1">
+    <row r="1" spans="1:55" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1680,94 +1688,97 @@
         <v>66</v>
       </c>
       <c r="Z1" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="AA1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AM1" s="23" t="s">
+      <c r="AN1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AN1" s="34" t="s">
+      <c r="AO1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="AO1" s="9" t="s">
+      <c r="AP1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AS1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AT1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AT1" s="32" t="s">
+      <c r="AU1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="AU1" s="33" t="s">
+      <c r="AV1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="AV1" s="27" t="s">
+      <c r="AW1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AX1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AX1" s="27" t="s">
+      <c r="AY1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AY1" s="27" t="s">
+      <c r="AZ1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="AZ1" s="27" t="s">
+      <c r="BA1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="BA1" s="31" t="s">
+      <c r="BB1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="BB1" s="31" t="s">
+      <c r="BC1" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:54">
+    <row r="2" spans="1:55">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1810,46 +1821,52 @@
       <c r="V2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="Z2" s="7" t="s">
+      <c r="Z2" s="7">
+        <v>4</v>
+      </c>
+      <c r="AA2" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AD2" s="2"/>
-      <c r="AF2" s="3" t="s">
+      <c r="AE2" s="2"/>
+      <c r="AG2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AH2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AR2" s="11" t="s">
+      <c r="AO2" s="5">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AV2" s="28"/>
       <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
       <c r="AZ2" s="28"/>
       <c r="BA2" s="28"/>
       <c r="BB2" s="28"/>
-    </row>
-    <row r="3" spans="1:54">
+      <c r="BC2" s="28"/>
+    </row>
+    <row r="3" spans="1:55">
       <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
@@ -1892,27 +1909,33 @@
       <c r="W3" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="AA3" s="35" t="s">
+      <c r="Z3" s="7">
+        <v>2</v>
+      </c>
+      <c r="AA3" s="7">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="AB3" s="3" t="s">
+      <c r="AC3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AR3" s="11" t="s">
+      <c r="AS3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="AV3" s="28"/>
       <c r="AW3" s="28"/>
       <c r="AX3" s="28"/>
       <c r="AY3" s="28"/>
       <c r="AZ3" s="28"/>
       <c r="BA3" s="28"/>
       <c r="BB3" s="28"/>
-    </row>
-    <row r="4" spans="1:54">
+      <c r="BC3" s="28"/>
+    </row>
+    <row r="4" spans="1:55">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -1961,21 +1984,21 @@
       <c r="V4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AK4" s="5" t="s">
+      <c r="AL4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AR4" s="11" t="s">
+      <c r="AS4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AV4" s="28"/>
       <c r="AW4" s="28"/>
       <c r="AX4" s="28"/>
       <c r="AY4" s="28"/>
       <c r="AZ4" s="28"/>
       <c r="BA4" s="28"/>
       <c r="BB4" s="28"/>
-    </row>
-    <row r="5" spans="1:54">
+      <c r="BC4" s="28"/>
+    </row>
+    <row r="5" spans="1:55">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -2015,30 +2038,30 @@
       <c r="W5" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="AA5" s="35" t="s">
+      <c r="AB5" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="AB5" s="3" t="s">
+      <c r="AC5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AD5" s="20" t="s">
+      <c r="AE5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="AK5" s="5" t="s">
+      <c r="AL5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AR5" s="11" t="s">
+      <c r="AS5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="AV5" s="28"/>
       <c r="AW5" s="28"/>
       <c r="AX5" s="28"/>
       <c r="AY5" s="28"/>
       <c r="AZ5" s="28"/>
       <c r="BA5" s="28"/>
       <c r="BB5" s="28"/>
-    </row>
-    <row r="6" spans="1:54">
+      <c r="BC5" s="28"/>
+    </row>
+    <row r="6" spans="1:55">
       <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
@@ -2087,21 +2110,21 @@
       <c r="W6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AK6" s="5" t="s">
+      <c r="AL6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AR6" s="11" t="s">
+      <c r="AS6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AV6" s="28"/>
       <c r="AW6" s="28"/>
       <c r="AX6" s="28"/>
       <c r="AY6" s="28"/>
       <c r="AZ6" s="28"/>
       <c r="BA6" s="28"/>
       <c r="BB6" s="28"/>
-    </row>
-    <row r="7" spans="1:54">
+      <c r="BC6" s="28"/>
+    </row>
+    <row r="7" spans="1:55">
       <c r="A7" s="14" t="s">
         <v>28</v>
       </c>
@@ -2135,21 +2158,21 @@
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
-      <c r="AK7" s="5" t="s">
+      <c r="AL7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AR7" s="11" t="s">
+      <c r="AS7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AV7" s="28"/>
       <c r="AW7" s="28"/>
       <c r="AX7" s="28"/>
       <c r="AY7" s="28"/>
       <c r="AZ7" s="28"/>
       <c r="BA7" s="28"/>
       <c r="BB7" s="28"/>
-    </row>
-    <row r="8" spans="1:54">
+      <c r="BC7" s="28"/>
+    </row>
+    <row r="8" spans="1:55">
       <c r="A8" s="14" t="s">
         <v>26</v>
       </c>
@@ -2199,21 +2222,21 @@
         <v>30</v>
       </c>
       <c r="W8" s="25"/>
-      <c r="AK8" s="5" t="s">
+      <c r="AL8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AR8" s="11" t="s">
+      <c r="AS8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AV8" s="28"/>
       <c r="AW8" s="28"/>
       <c r="AX8" s="28"/>
       <c r="AY8" s="28"/>
       <c r="AZ8" s="28"/>
       <c r="BA8" s="28"/>
       <c r="BB8" s="28"/>
-    </row>
-    <row r="9" spans="1:54">
+      <c r="BC8" s="28"/>
+    </row>
+    <row r="9" spans="1:55">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -2258,30 +2281,30 @@
       <c r="W9" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AA9" s="35" t="s">
+      <c r="AB9" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="AB9" s="3" t="s">
+      <c r="AC9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AD9" s="21" t="s">
+      <c r="AE9" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="AK9" s="23" t="s">
+      <c r="AL9" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AR9" s="11" t="s">
+      <c r="AS9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AV9" s="28"/>
       <c r="AW9" s="28"/>
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="28"/>
       <c r="BB9" s="28"/>
-    </row>
-    <row r="10" spans="1:54">
+      <c r="BC9" s="28"/>
+    </row>
+    <row r="10" spans="1:55">
       <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
@@ -2326,21 +2349,21 @@
       <c r="W10" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AK10" s="5" t="s">
+      <c r="AL10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AR10" s="11" t="s">
+      <c r="AS10" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="AV10" s="28"/>
       <c r="AW10" s="28"/>
       <c r="AX10" s="28"/>
       <c r="AY10" s="28"/>
       <c r="AZ10" s="28"/>
       <c r="BA10" s="28"/>
       <c r="BB10" s="28"/>
-    </row>
-    <row r="11" spans="1:54">
+      <c r="BC10" s="28"/>
+    </row>
+    <row r="11" spans="1:55">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
@@ -2374,21 +2397,21 @@
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="AK11" s="5" t="s">
+      <c r="AL11" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AR11" s="11" t="s">
+      <c r="AS11" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AV11" s="28"/>
       <c r="AW11" s="28"/>
       <c r="AX11" s="28"/>
       <c r="AY11" s="28"/>
       <c r="AZ11" s="28"/>
       <c r="BA11" s="28"/>
       <c r="BB11" s="28"/>
-    </row>
-    <row r="12" spans="1:54">
+      <c r="BC11" s="28"/>
+    </row>
+    <row r="12" spans="1:55">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -2428,24 +2451,24 @@
       <c r="O12" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="AA12" s="35" t="s">
+      <c r="AB12" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="AK12" s="5" t="s">
+      <c r="AL12" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AR12" s="11" t="s">
+      <c r="AS12" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="AV12" s="28"/>
       <c r="AW12" s="28"/>
       <c r="AX12" s="28"/>
       <c r="AY12" s="28"/>
       <c r="AZ12" s="28"/>
       <c r="BA12" s="28"/>
       <c r="BB12" s="28"/>
-    </row>
-    <row r="13" spans="1:54">
+      <c r="BC12" s="28"/>
+    </row>
+    <row r="13" spans="1:55">
       <c r="A13" s="14" t="s">
         <v>79</v>
       </c>
@@ -2485,21 +2508,21 @@
       <c r="O13" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="AK13" s="5" t="s">
+      <c r="AL13" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="AR13" s="11" t="s">
+      <c r="AS13" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="AV13" s="28"/>
       <c r="AW13" s="28"/>
       <c r="AX13" s="28"/>
       <c r="AY13" s="28"/>
       <c r="AZ13" s="28"/>
       <c r="BA13" s="28"/>
       <c r="BB13" s="28"/>
-    </row>
-    <row r="14" spans="1:54" ht="13" customHeight="1">
+      <c r="BC13" s="28"/>
+    </row>
+    <row r="14" spans="1:55" ht="12.95" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -2533,21 +2556,21 @@
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
-      <c r="AK14" s="5" t="s">
+      <c r="AL14" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AR14" s="11" t="s">
+      <c r="AS14" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AV14" s="28"/>
       <c r="AW14" s="28"/>
       <c r="AX14" s="28"/>
       <c r="AY14" s="28"/>
       <c r="AZ14" s="28"/>
       <c r="BA14" s="28"/>
       <c r="BB14" s="28"/>
-    </row>
-    <row r="15" spans="1:54">
+      <c r="BC14" s="28"/>
+    </row>
+    <row r="15" spans="1:55">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
@@ -2581,21 +2604,21 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-      <c r="AK15" s="5" t="s">
+      <c r="AL15" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AR15" s="11" t="s">
+      <c r="AS15" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="AV15" s="28"/>
       <c r="AW15" s="28"/>
       <c r="AX15" s="28"/>
       <c r="AY15" s="28"/>
       <c r="AZ15" s="28"/>
       <c r="BA15" s="28"/>
       <c r="BB15" s="28"/>
-    </row>
-    <row r="16" spans="1:54">
+      <c r="BC15" s="28"/>
+    </row>
+    <row r="16" spans="1:55">
       <c r="A16" s="14" t="s">
         <v>32</v>
       </c>
@@ -2640,38 +2663,38 @@
       <c r="W16" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AA16" s="35" t="s">
+      <c r="AB16" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="AB16" s="3" t="s">
+      <c r="AC16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AD16" s="2" t="s">
+      <c r="AE16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AH16" s="37" t="s">
+      <c r="AI16" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="AI16" s="22" t="s">
+      <c r="AJ16" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="AJ16" s="5" t="s">
+      <c r="AK16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AK16" s="15"/>
-      <c r="AP16" s="18"/>
-      <c r="AR16" s="9" t="s">
+      <c r="AL16" s="15"/>
+      <c r="AQ16" s="18"/>
+      <c r="AS16" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AV16" s="28"/>
-      <c r="AW16" s="29"/>
-      <c r="AX16" s="28"/>
+      <c r="AW16" s="28"/>
+      <c r="AX16" s="29"/>
       <c r="AY16" s="28"/>
       <c r="AZ16" s="28"/>
       <c r="BA16" s="28"/>
       <c r="BB16" s="28"/>
-    </row>
-    <row r="17" spans="1:54">
+      <c r="BC16" s="28"/>
+    </row>
+    <row r="17" spans="1:55">
       <c r="A17" s="14" t="s">
         <v>80</v>
       </c>
@@ -2714,20 +2737,20 @@
       <c r="W17" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AI17" s="22"/>
-      <c r="AP17" s="18"/>
-      <c r="AR17" s="11" t="s">
+      <c r="AJ17" s="22"/>
+      <c r="AQ17" s="18"/>
+      <c r="AS17" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="AV17" s="28"/>
-      <c r="AW17" s="29"/>
-      <c r="AX17" s="28"/>
+      <c r="AW17" s="28"/>
+      <c r="AX17" s="29"/>
       <c r="AY17" s="28"/>
       <c r="AZ17" s="28"/>
       <c r="BA17" s="28"/>
       <c r="BB17" s="28"/>
-    </row>
-    <row r="18" spans="1:54">
+      <c r="BC17" s="28"/>
+    </row>
+    <row r="18" spans="1:55">
       <c r="A18" s="14" t="s">
         <v>63</v>
       </c>
@@ -2774,28 +2797,28 @@
         <v>64</v>
       </c>
       <c r="W18" s="16"/>
-      <c r="AA18" s="35" t="s">
+      <c r="AB18" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="AB18" s="3" t="s">
+      <c r="AC18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AD18" s="2" t="s">
+      <c r="AE18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AK18" s="4"/>
-      <c r="AR18" s="11" t="s">
+      <c r="AL18" s="4"/>
+      <c r="AS18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="AV18" s="28"/>
       <c r="AW18" s="28"/>
       <c r="AX18" s="28"/>
       <c r="AY18" s="28"/>
       <c r="AZ18" s="28"/>
       <c r="BA18" s="28"/>
       <c r="BB18" s="28"/>
-    </row>
-    <row r="19" spans="1:54">
+      <c r="BC18" s="28"/>
+    </row>
+    <row r="19" spans="1:55">
       <c r="A19" s="14" t="s">
         <v>81</v>
       </c>
@@ -2840,37 +2863,37 @@
       <c r="W19" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AA19" s="35" t="s">
+      <c r="AB19" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="AB19" s="5" t="s">
+      <c r="AC19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AC19" s="5" t="s">
+      <c r="AD19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AD19" s="39"/>
-      <c r="AH19" s="37" t="s">
+      <c r="AE19" s="39"/>
+      <c r="AI19" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="AI19" s="5" t="s">
+      <c r="AJ19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AK19" s="26" t="s">
+      <c r="AL19" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AR19" s="11" t="s">
+      <c r="AS19" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="AV19" s="28"/>
       <c r="AW19" s="28"/>
       <c r="AX19" s="28"/>
       <c r="AY19" s="28"/>
       <c r="AZ19" s="28"/>
       <c r="BA19" s="28"/>
       <c r="BB19" s="28"/>
-    </row>
-    <row r="20" spans="1:54">
+      <c r="BC19" s="28"/>
+    </row>
+    <row r="20" spans="1:55">
       <c r="A20" s="19" t="s">
         <v>64</v>
       </c>
@@ -2913,16 +2936,16 @@
       <c r="W20" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AK20" s="4"/>
-      <c r="AV20" s="28"/>
+      <c r="AL20" s="4"/>
       <c r="AW20" s="28"/>
       <c r="AX20" s="28"/>
       <c r="AY20" s="28"/>
       <c r="AZ20" s="28"/>
       <c r="BA20" s="28"/>
       <c r="BB20" s="28"/>
-    </row>
-    <row r="21" spans="1:54">
+      <c r="BC20" s="28"/>
+    </row>
+    <row r="21" spans="1:55">
       <c r="A21" s="14" t="s">
         <v>105</v>
       </c>
@@ -2950,396 +2973,396 @@
       <c r="M21" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="AV21" s="28"/>
       <c r="AW21" s="28"/>
       <c r="AX21" s="28"/>
       <c r="AY21" s="28"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="28"/>
       <c r="BB21" s="28"/>
-    </row>
-    <row r="22" spans="1:54">
+      <c r="BC21" s="28"/>
+    </row>
+    <row r="22" spans="1:55">
       <c r="M22" s="15"/>
-      <c r="AV22" s="28"/>
       <c r="AW22" s="28"/>
       <c r="AX22" s="28"/>
       <c r="AY22" s="28"/>
       <c r="AZ22" s="28"/>
       <c r="BA22" s="28"/>
       <c r="BB22" s="28"/>
-    </row>
-    <row r="23" spans="1:54">
-      <c r="AV23" s="28"/>
+      <c r="BC22" s="28"/>
+    </row>
+    <row r="23" spans="1:55">
       <c r="AW23" s="28"/>
       <c r="AX23" s="28"/>
       <c r="AY23" s="28"/>
       <c r="AZ23" s="28"/>
       <c r="BA23" s="28"/>
       <c r="BB23" s="28"/>
-    </row>
-    <row r="24" spans="1:54">
-      <c r="AV24" s="28"/>
+      <c r="BC23" s="28"/>
+    </row>
+    <row r="24" spans="1:55">
       <c r="AW24" s="28"/>
       <c r="AX24" s="28"/>
       <c r="AY24" s="28"/>
       <c r="AZ24" s="28"/>
       <c r="BA24" s="28"/>
       <c r="BB24" s="28"/>
-    </row>
-    <row r="25" spans="1:54">
-      <c r="AV25" s="28"/>
+      <c r="BC24" s="28"/>
+    </row>
+    <row r="25" spans="1:55">
       <c r="AW25" s="28"/>
       <c r="AX25" s="28"/>
       <c r="AY25" s="28"/>
       <c r="AZ25" s="28"/>
       <c r="BA25" s="28"/>
       <c r="BB25" s="28"/>
-    </row>
-    <row r="26" spans="1:54">
-      <c r="AV26" s="28"/>
+      <c r="BC25" s="28"/>
+    </row>
+    <row r="26" spans="1:55">
       <c r="AW26" s="28"/>
       <c r="AX26" s="28"/>
       <c r="AY26" s="28"/>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="28"/>
       <c r="BB26" s="28"/>
-    </row>
-    <row r="27" spans="1:54">
-      <c r="AV27" s="28"/>
+      <c r="BC26" s="28"/>
+    </row>
+    <row r="27" spans="1:55">
       <c r="AW27" s="28"/>
       <c r="AX27" s="28"/>
       <c r="AY27" s="28"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="28"/>
       <c r="BB27" s="28"/>
-    </row>
-    <row r="28" spans="1:54">
-      <c r="AV28" s="28"/>
+      <c r="BC27" s="28"/>
+    </row>
+    <row r="28" spans="1:55">
       <c r="AW28" s="28"/>
       <c r="AX28" s="28"/>
       <c r="AY28" s="28"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="28"/>
       <c r="BB28" s="28"/>
-    </row>
-    <row r="29" spans="1:54">
-      <c r="AV29" s="28"/>
+      <c r="BC28" s="28"/>
+    </row>
+    <row r="29" spans="1:55">
       <c r="AW29" s="28"/>
       <c r="AX29" s="28"/>
       <c r="AY29" s="28"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="28"/>
       <c r="BB29" s="28"/>
-    </row>
-    <row r="30" spans="1:54">
-      <c r="AV30" s="28"/>
+      <c r="BC29" s="28"/>
+    </row>
+    <row r="30" spans="1:55">
       <c r="AW30" s="28"/>
       <c r="AX30" s="28"/>
       <c r="AY30" s="28"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="28"/>
       <c r="BB30" s="28"/>
-    </row>
-    <row r="31" spans="1:54">
-      <c r="AV31" s="28"/>
+      <c r="BC30" s="28"/>
+    </row>
+    <row r="31" spans="1:55">
       <c r="AW31" s="28"/>
       <c r="AX31" s="28"/>
       <c r="AY31" s="28"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="28"/>
       <c r="BB31" s="28"/>
-    </row>
-    <row r="32" spans="1:54">
-      <c r="AV32" s="28"/>
+      <c r="BC31" s="28"/>
+    </row>
+    <row r="32" spans="1:55">
       <c r="AW32" s="28"/>
       <c r="AX32" s="28"/>
       <c r="AY32" s="28"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="28"/>
       <c r="BB32" s="28"/>
-    </row>
-    <row r="33" spans="48:54">
-      <c r="AV33" s="24"/>
+      <c r="BC32" s="28"/>
+    </row>
+    <row r="33" spans="49:55">
       <c r="AW33" s="24"/>
       <c r="AX33" s="24"/>
       <c r="AY33" s="24"/>
       <c r="AZ33" s="24"/>
       <c r="BA33" s="24"/>
       <c r="BB33" s="24"/>
-    </row>
-    <row r="34" spans="48:54">
-      <c r="AV34" s="24"/>
+      <c r="BC33" s="24"/>
+    </row>
+    <row r="34" spans="49:55">
       <c r="AW34" s="24"/>
       <c r="AX34" s="24"/>
       <c r="AY34" s="24"/>
       <c r="AZ34" s="24"/>
       <c r="BA34" s="24"/>
       <c r="BB34" s="24"/>
-    </row>
-    <row r="35" spans="48:54">
-      <c r="AV35" s="24"/>
+      <c r="BC34" s="24"/>
+    </row>
+    <row r="35" spans="49:55">
       <c r="AW35" s="24"/>
       <c r="AX35" s="24"/>
       <c r="AY35" s="24"/>
       <c r="AZ35" s="24"/>
       <c r="BA35" s="24"/>
       <c r="BB35" s="24"/>
-    </row>
-    <row r="36" spans="48:54">
-      <c r="AV36" s="24"/>
+      <c r="BC35" s="24"/>
+    </row>
+    <row r="36" spans="49:55">
       <c r="AW36" s="24"/>
       <c r="AX36" s="24"/>
       <c r="AY36" s="24"/>
       <c r="AZ36" s="24"/>
       <c r="BA36" s="24"/>
       <c r="BB36" s="24"/>
-    </row>
-    <row r="37" spans="48:54">
-      <c r="AV37" s="24"/>
+      <c r="BC36" s="24"/>
+    </row>
+    <row r="37" spans="49:55">
       <c r="AW37" s="24"/>
       <c r="AX37" s="24"/>
       <c r="AY37" s="24"/>
       <c r="AZ37" s="24"/>
       <c r="BA37" s="24"/>
       <c r="BB37" s="24"/>
-    </row>
-    <row r="38" spans="48:54">
-      <c r="AV38" s="24"/>
+      <c r="BC37" s="24"/>
+    </row>
+    <row r="38" spans="49:55">
       <c r="AW38" s="24"/>
       <c r="AX38" s="24"/>
       <c r="AY38" s="24"/>
       <c r="AZ38" s="24"/>
       <c r="BA38" s="24"/>
       <c r="BB38" s="24"/>
-    </row>
-    <row r="39" spans="48:54">
-      <c r="AV39" s="24"/>
+      <c r="BC38" s="24"/>
+    </row>
+    <row r="39" spans="49:55">
       <c r="AW39" s="24"/>
       <c r="AX39" s="24"/>
       <c r="AY39" s="24"/>
       <c r="AZ39" s="24"/>
       <c r="BA39" s="24"/>
       <c r="BB39" s="24"/>
-    </row>
-    <row r="40" spans="48:54">
-      <c r="AV40" s="24"/>
+      <c r="BC39" s="24"/>
+    </row>
+    <row r="40" spans="49:55">
       <c r="AW40" s="24"/>
       <c r="AX40" s="24"/>
       <c r="AY40" s="24"/>
       <c r="AZ40" s="24"/>
       <c r="BA40" s="24"/>
       <c r="BB40" s="24"/>
-    </row>
-    <row r="41" spans="48:54">
-      <c r="AV41" s="24"/>
+      <c r="BC40" s="24"/>
+    </row>
+    <row r="41" spans="49:55">
       <c r="AW41" s="24"/>
       <c r="AX41" s="24"/>
       <c r="AY41" s="24"/>
       <c r="AZ41" s="24"/>
       <c r="BA41" s="24"/>
       <c r="BB41" s="24"/>
-    </row>
-    <row r="42" spans="48:54">
-      <c r="AV42" s="24"/>
+      <c r="BC41" s="24"/>
+    </row>
+    <row r="42" spans="49:55">
       <c r="AW42" s="24"/>
       <c r="AX42" s="24"/>
       <c r="AY42" s="24"/>
       <c r="AZ42" s="24"/>
       <c r="BA42" s="24"/>
       <c r="BB42" s="24"/>
-    </row>
-    <row r="43" spans="48:54">
-      <c r="AV43" s="24"/>
+      <c r="BC42" s="24"/>
+    </row>
+    <row r="43" spans="49:55">
       <c r="AW43" s="24"/>
       <c r="AX43" s="24"/>
       <c r="AY43" s="24"/>
       <c r="AZ43" s="24"/>
       <c r="BA43" s="24"/>
       <c r="BB43" s="24"/>
-    </row>
-    <row r="44" spans="48:54">
-      <c r="AV44" s="24"/>
+      <c r="BC43" s="24"/>
+    </row>
+    <row r="44" spans="49:55">
       <c r="AW44" s="24"/>
       <c r="AX44" s="24"/>
       <c r="AY44" s="24"/>
       <c r="AZ44" s="24"/>
       <c r="BA44" s="24"/>
       <c r="BB44" s="24"/>
-    </row>
-    <row r="45" spans="48:54">
-      <c r="AV45" s="24"/>
+      <c r="BC44" s="24"/>
+    </row>
+    <row r="45" spans="49:55">
       <c r="AW45" s="24"/>
       <c r="AX45" s="24"/>
       <c r="AY45" s="24"/>
       <c r="AZ45" s="24"/>
       <c r="BA45" s="24"/>
       <c r="BB45" s="24"/>
-    </row>
-    <row r="46" spans="48:54">
-      <c r="AV46" s="24"/>
+      <c r="BC45" s="24"/>
+    </row>
+    <row r="46" spans="49:55">
       <c r="AW46" s="24"/>
       <c r="AX46" s="24"/>
       <c r="AY46" s="24"/>
       <c r="AZ46" s="24"/>
       <c r="BA46" s="24"/>
       <c r="BB46" s="24"/>
-    </row>
-    <row r="47" spans="48:54">
-      <c r="AV47" s="24"/>
+      <c r="BC46" s="24"/>
+    </row>
+    <row r="47" spans="49:55">
       <c r="AW47" s="24"/>
       <c r="AX47" s="24"/>
       <c r="AY47" s="24"/>
       <c r="AZ47" s="24"/>
       <c r="BA47" s="24"/>
       <c r="BB47" s="24"/>
-    </row>
-    <row r="48" spans="48:54">
-      <c r="AV48" s="24"/>
+      <c r="BC47" s="24"/>
+    </row>
+    <row r="48" spans="49:55">
       <c r="AW48" s="24"/>
       <c r="AX48" s="24"/>
       <c r="AY48" s="24"/>
       <c r="AZ48" s="24"/>
       <c r="BA48" s="24"/>
       <c r="BB48" s="24"/>
-    </row>
-    <row r="49" spans="48:54">
-      <c r="AV49" s="24"/>
+      <c r="BC48" s="24"/>
+    </row>
+    <row r="49" spans="49:55">
       <c r="AW49" s="24"/>
       <c r="AX49" s="24"/>
       <c r="AY49" s="24"/>
       <c r="AZ49" s="24"/>
       <c r="BA49" s="24"/>
       <c r="BB49" s="24"/>
-    </row>
-    <row r="50" spans="48:54">
-      <c r="AV50" s="24"/>
+      <c r="BC49" s="24"/>
+    </row>
+    <row r="50" spans="49:55">
       <c r="AW50" s="24"/>
       <c r="AX50" s="24"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="24"/>
       <c r="BA50" s="24"/>
       <c r="BB50" s="24"/>
-    </row>
-    <row r="51" spans="48:54">
-      <c r="AV51" s="24"/>
+      <c r="BC50" s="24"/>
+    </row>
+    <row r="51" spans="49:55">
       <c r="AW51" s="24"/>
       <c r="AX51" s="24"/>
       <c r="AY51" s="24"/>
       <c r="AZ51" s="24"/>
       <c r="BA51" s="24"/>
       <c r="BB51" s="24"/>
-    </row>
-    <row r="52" spans="48:54">
-      <c r="AV52" s="24"/>
+      <c r="BC51" s="24"/>
+    </row>
+    <row r="52" spans="49:55">
       <c r="AW52" s="24"/>
       <c r="AX52" s="24"/>
       <c r="AY52" s="24"/>
       <c r="AZ52" s="24"/>
       <c r="BA52" s="24"/>
       <c r="BB52" s="24"/>
-    </row>
-    <row r="53" spans="48:54">
-      <c r="AV53" s="24"/>
+      <c r="BC52" s="24"/>
+    </row>
+    <row r="53" spans="49:55">
       <c r="AW53" s="24"/>
       <c r="AX53" s="24"/>
       <c r="AY53" s="24"/>
       <c r="AZ53" s="24"/>
       <c r="BA53" s="24"/>
       <c r="BB53" s="24"/>
-    </row>
-    <row r="54" spans="48:54">
-      <c r="AV54" s="24"/>
+      <c r="BC53" s="24"/>
+    </row>
+    <row r="54" spans="49:55">
       <c r="AW54" s="24"/>
       <c r="AX54" s="24"/>
       <c r="AY54" s="24"/>
       <c r="AZ54" s="24"/>
       <c r="BA54" s="24"/>
       <c r="BB54" s="24"/>
-    </row>
-    <row r="55" spans="48:54">
-      <c r="AV55" s="24"/>
+      <c r="BC54" s="24"/>
+    </row>
+    <row r="55" spans="49:55">
       <c r="AW55" s="24"/>
       <c r="AX55" s="24"/>
       <c r="AY55" s="24"/>
       <c r="AZ55" s="24"/>
       <c r="BA55" s="24"/>
       <c r="BB55" s="24"/>
-    </row>
-    <row r="56" spans="48:54">
-      <c r="AV56" s="24"/>
+      <c r="BC55" s="24"/>
+    </row>
+    <row r="56" spans="49:55">
       <c r="AW56" s="24"/>
       <c r="AX56" s="24"/>
       <c r="AY56" s="24"/>
       <c r="AZ56" s="24"/>
       <c r="BA56" s="24"/>
       <c r="BB56" s="24"/>
-    </row>
-    <row r="57" spans="48:54">
-      <c r="AV57" s="24"/>
+      <c r="BC56" s="24"/>
+    </row>
+    <row r="57" spans="49:55">
       <c r="AW57" s="24"/>
       <c r="AX57" s="24"/>
       <c r="AY57" s="24"/>
       <c r="AZ57" s="24"/>
       <c r="BA57" s="24"/>
       <c r="BB57" s="24"/>
-    </row>
-    <row r="58" spans="48:54">
-      <c r="AV58" s="24"/>
+      <c r="BC57" s="24"/>
+    </row>
+    <row r="58" spans="49:55">
       <c r="AW58" s="24"/>
       <c r="AX58" s="24"/>
       <c r="AY58" s="24"/>
       <c r="AZ58" s="24"/>
       <c r="BA58" s="24"/>
       <c r="BB58" s="24"/>
-    </row>
-    <row r="59" spans="48:54">
-      <c r="AV59" s="24"/>
+      <c r="BC58" s="24"/>
+    </row>
+    <row r="59" spans="49:55">
       <c r="AW59" s="24"/>
       <c r="AX59" s="24"/>
       <c r="AY59" s="24"/>
       <c r="AZ59" s="24"/>
       <c r="BA59" s="24"/>
       <c r="BB59" s="24"/>
-    </row>
-    <row r="60" spans="48:54">
-      <c r="BA60" s="11"/>
+      <c r="BC59" s="24"/>
+    </row>
+    <row r="60" spans="49:55">
       <c r="BB60" s="11"/>
-    </row>
-    <row r="61" spans="48:54">
-      <c r="BA61" s="11"/>
+      <c r="BC60" s="11"/>
+    </row>
+    <row r="61" spans="49:55">
       <c r="BB61" s="11"/>
-    </row>
-    <row r="62" spans="48:54">
-      <c r="BA62" s="11"/>
+      <c r="BC61" s="11"/>
+    </row>
+    <row r="62" spans="49:55">
       <c r="BB62" s="11"/>
-    </row>
-    <row r="63" spans="48:54">
-      <c r="BA63" s="11"/>
+      <c r="BC62" s="11"/>
+    </row>
+    <row r="63" spans="49:55">
       <c r="BB63" s="11"/>
-    </row>
-    <row r="64" spans="48:54">
-      <c r="BA64" s="11"/>
+      <c r="BC63" s="11"/>
+    </row>
+    <row r="64" spans="49:55">
       <c r="BB64" s="11"/>
-    </row>
-    <row r="65" spans="53:54">
-      <c r="BA65" s="11"/>
+      <c r="BC64" s="11"/>
+    </row>
+    <row r="65" spans="54:55">
       <c r="BB65" s="11"/>
-    </row>
-    <row r="66" spans="53:54">
-      <c r="BA66" s="11"/>
+      <c r="BC65" s="11"/>
+    </row>
+    <row r="66" spans="54:55">
       <c r="BB66" s="11"/>
-    </row>
-    <row r="67" spans="53:54">
-      <c r="BA67" s="11"/>
+      <c r="BC66" s="11"/>
+    </row>
+    <row r="67" spans="54:55">
       <c r="BB67" s="11"/>
-    </row>
-    <row r="68" spans="53:54">
-      <c r="BA68" s="11"/>
+      <c r="BC67" s="11"/>
+    </row>
+    <row r="68" spans="54:55">
       <c r="BB68" s="11"/>
+      <c r="BC68" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="AC5:AE6">
-    <sortCondition descending="1" ref="AE5"/>
+  <sortState ref="AD5:AF6">
+    <sortCondition descending="1" ref="AF5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>

<commit_message>
added app column -> vEvent message to config
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine2.xlsx
+++ b/scoretools/test/mkGameEngine2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="153">
   <si>
     <t>stage</t>
   </si>
@@ -477,6 +477,15 @@
   </si>
   <si>
     <t>v.mc.delay</t>
+  </si>
+  <si>
+    <t>app</t>
+  </si>
+  <si>
+    <t>success</t>
+  </si>
+  <si>
+    <t>test:123</t>
   </si>
 </sst>
 </file>
@@ -1554,10 +1563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BC68"/>
+  <dimension ref="A1:BD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AP2" sqref="AP2"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AB4" sqref="AB4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1586,32 +1595,33 @@
     <col min="24" max="24" width="8.28515625" style="7" customWidth="1"/>
     <col min="25" max="26" width="9.42578125" style="7" customWidth="1"/>
     <col min="27" max="27" width="12.140625" style="7" customWidth="1"/>
-    <col min="28" max="28" width="24" style="3" customWidth="1"/>
-    <col min="29" max="29" width="11.140625" style="3" customWidth="1"/>
-    <col min="30" max="30" width="8.28515625" style="3" customWidth="1"/>
-    <col min="31" max="31" width="6.85546875" style="3" customWidth="1"/>
-    <col min="32" max="32" width="8.85546875" style="3"/>
-    <col min="33" max="33" width="14.7109375" style="3" customWidth="1"/>
-    <col min="34" max="34" width="9.28515625" style="3" customWidth="1"/>
-    <col min="35" max="35" width="19.28515625" style="5" customWidth="1"/>
-    <col min="36" max="36" width="11" style="5" customWidth="1"/>
-    <col min="37" max="37" width="6.85546875" style="5" customWidth="1"/>
-    <col min="38" max="38" width="6.7109375" style="5" customWidth="1"/>
-    <col min="39" max="41" width="8.85546875" style="5"/>
-    <col min="42" max="42" width="13" style="11" customWidth="1"/>
-    <col min="43" max="43" width="20.140625" style="11" customWidth="1"/>
-    <col min="44" max="44" width="6.42578125" style="11" customWidth="1"/>
-    <col min="45" max="45" width="6.7109375" style="11" customWidth="1"/>
-    <col min="46" max="48" width="8.85546875" style="11"/>
-    <col min="49" max="49" width="20.7109375" style="11" customWidth="1"/>
-    <col min="50" max="50" width="20.140625" style="11" customWidth="1"/>
-    <col min="51" max="51" width="6.42578125" style="11" customWidth="1"/>
-    <col min="52" max="52" width="6.7109375" style="11" customWidth="1"/>
-    <col min="53" max="53" width="8.85546875" style="11"/>
-    <col min="54" max="55" width="8.85546875" style="30"/>
+    <col min="28" max="28" width="10.85546875" style="7" customWidth="1"/>
+    <col min="29" max="29" width="24" style="3" customWidth="1"/>
+    <col min="30" max="30" width="11.140625" style="3" customWidth="1"/>
+    <col min="31" max="31" width="8.28515625" style="3" customWidth="1"/>
+    <col min="32" max="32" width="6.85546875" style="3" customWidth="1"/>
+    <col min="33" max="33" width="8.85546875" style="3"/>
+    <col min="34" max="34" width="14.7109375" style="3" customWidth="1"/>
+    <col min="35" max="35" width="9.28515625" style="3" customWidth="1"/>
+    <col min="36" max="36" width="19.28515625" style="5" customWidth="1"/>
+    <col min="37" max="37" width="11" style="5" customWidth="1"/>
+    <col min="38" max="38" width="6.85546875" style="5" customWidth="1"/>
+    <col min="39" max="39" width="6.7109375" style="5" customWidth="1"/>
+    <col min="40" max="42" width="8.85546875" style="5"/>
+    <col min="43" max="43" width="13" style="11" customWidth="1"/>
+    <col min="44" max="44" width="20.140625" style="11" customWidth="1"/>
+    <col min="45" max="45" width="6.42578125" style="11" customWidth="1"/>
+    <col min="46" max="46" width="6.7109375" style="11" customWidth="1"/>
+    <col min="47" max="49" width="8.85546875" style="11"/>
+    <col min="50" max="50" width="20.7109375" style="11" customWidth="1"/>
+    <col min="51" max="51" width="20.140625" style="11" customWidth="1"/>
+    <col min="52" max="52" width="6.42578125" style="11" customWidth="1"/>
+    <col min="53" max="53" width="6.7109375" style="11" customWidth="1"/>
+    <col min="54" max="54" width="8.85546875" style="11"/>
+    <col min="55" max="56" width="8.85546875" style="30"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="1" customFormat="1">
+    <row r="1" spans="1:56" s="1" customFormat="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1693,92 +1703,95 @@
       <c r="AA1" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AB1" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="AC1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="AN1" s="23" t="s">
+      <c r="AO1" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="AO1" s="34" t="s">
+      <c r="AP1" s="34" t="s">
         <v>67</v>
       </c>
-      <c r="AP1" s="9" t="s">
+      <c r="AQ1" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="AQ1" s="9" t="s">
+      <c r="AR1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="AR1" s="9" t="s">
+      <c r="AS1" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="AS1" s="9" t="s">
+      <c r="AT1" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="AT1" s="9" t="s">
+      <c r="AU1" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="AU1" s="32" t="s">
+      <c r="AV1" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="AV1" s="33" t="s">
+      <c r="AW1" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="AW1" s="27" t="s">
+      <c r="AX1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="AX1" s="27" t="s">
+      <c r="AY1" s="27" t="s">
         <v>17</v>
       </c>
-      <c r="AY1" s="27" t="s">
+      <c r="AZ1" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="AZ1" s="27" t="s">
+      <c r="BA1" s="27" t="s">
         <v>20</v>
       </c>
-      <c r="BA1" s="27" t="s">
+      <c r="BB1" s="27" t="s">
         <v>15</v>
       </c>
-      <c r="BB1" s="31" t="s">
+      <c r="BC1" s="31" t="s">
         <v>66</v>
       </c>
-      <c r="BC1" s="31" t="s">
+      <c r="BD1" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:55">
+    <row r="2" spans="1:56">
       <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
@@ -1827,46 +1840,49 @@
       <c r="AA2" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AB2" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="AC2" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="2"/>
-      <c r="AG2" s="3" t="s">
+      <c r="AF2" s="2"/>
+      <c r="AH2" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AK2" s="5" t="s">
+      <c r="AL2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AO2" s="5">
+      <c r="AP2" s="5">
         <v>1</v>
       </c>
-      <c r="AS2" s="11" t="s">
+      <c r="AT2" s="11" t="s">
         <v>52</v>
       </c>
-      <c r="AW2" s="28"/>
       <c r="AX2" s="28"/>
       <c r="AY2" s="28"/>
       <c r="AZ2" s="28"/>
       <c r="BA2" s="28"/>
       <c r="BB2" s="28"/>
       <c r="BC2" s="28"/>
-    </row>
-    <row r="3" spans="1:55">
+      <c r="BD2" s="28"/>
+    </row>
+    <row r="3" spans="1:56">
       <c r="A3" s="14" t="s">
         <v>25</v>
       </c>
@@ -1915,27 +1931,27 @@
       <c r="AA3" s="7">
         <v>1</v>
       </c>
-      <c r="AB3" s="35" t="s">
+      <c r="AC3" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="AC3" s="3" t="s">
+      <c r="AD3" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="AD3" s="3" t="s">
+      <c r="AE3" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AS3" s="11" t="s">
+      <c r="AT3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="AW3" s="28"/>
       <c r="AX3" s="28"/>
       <c r="AY3" s="28"/>
       <c r="AZ3" s="28"/>
       <c r="BA3" s="28"/>
       <c r="BB3" s="28"/>
       <c r="BC3" s="28"/>
-    </row>
-    <row r="4" spans="1:55">
+      <c r="BD3" s="28"/>
+    </row>
+    <row r="4" spans="1:56">
       <c r="A4" s="14" t="s">
         <v>4</v>
       </c>
@@ -1984,21 +2000,24 @@
       <c r="V4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="AL4" s="5" t="s">
+      <c r="AB4" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="AM4" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="AS4" s="11" t="s">
+      <c r="AT4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="AW4" s="28"/>
       <c r="AX4" s="28"/>
       <c r="AY4" s="28"/>
       <c r="AZ4" s="28"/>
       <c r="BA4" s="28"/>
       <c r="BB4" s="28"/>
       <c r="BC4" s="28"/>
-    </row>
-    <row r="5" spans="1:55">
+      <c r="BD4" s="28"/>
+    </row>
+    <row r="5" spans="1:56">
       <c r="A5" s="14" t="s">
         <v>6</v>
       </c>
@@ -2038,30 +2057,30 @@
       <c r="W5" s="17" t="s">
         <v>127</v>
       </c>
-      <c r="AB5" s="35" t="s">
+      <c r="AC5" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="AC5" s="3" t="s">
+      <c r="AD5" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="AE5" s="20" t="s">
+      <c r="AF5" s="20" t="s">
         <v>127</v>
       </c>
-      <c r="AL5" s="5" t="s">
+      <c r="AM5" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AS5" s="11" t="s">
+      <c r="AT5" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="AW5" s="28"/>
       <c r="AX5" s="28"/>
       <c r="AY5" s="28"/>
       <c r="AZ5" s="28"/>
       <c r="BA5" s="28"/>
       <c r="BB5" s="28"/>
       <c r="BC5" s="28"/>
-    </row>
-    <row r="6" spans="1:55">
+      <c r="BD5" s="28"/>
+    </row>
+    <row r="6" spans="1:56">
       <c r="A6" s="14" t="s">
         <v>27</v>
       </c>
@@ -2110,21 +2129,21 @@
       <c r="W6" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AL6" s="5" t="s">
+      <c r="AM6" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="AS6" s="11" t="s">
+      <c r="AT6" s="11" t="s">
         <v>113</v>
       </c>
-      <c r="AW6" s="28"/>
       <c r="AX6" s="28"/>
       <c r="AY6" s="28"/>
       <c r="AZ6" s="28"/>
       <c r="BA6" s="28"/>
       <c r="BB6" s="28"/>
       <c r="BC6" s="28"/>
-    </row>
-    <row r="7" spans="1:55">
+      <c r="BD6" s="28"/>
+    </row>
+    <row r="7" spans="1:56">
       <c r="A7" s="14" t="s">
         <v>28</v>
       </c>
@@ -2158,21 +2177,21 @@
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
       <c r="O7" s="15"/>
-      <c r="AL7" s="5" t="s">
+      <c r="AM7" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AS7" s="11" t="s">
+      <c r="AT7" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="AW7" s="28"/>
       <c r="AX7" s="28"/>
       <c r="AY7" s="28"/>
       <c r="AZ7" s="28"/>
       <c r="BA7" s="28"/>
       <c r="BB7" s="28"/>
       <c r="BC7" s="28"/>
-    </row>
-    <row r="8" spans="1:55">
+      <c r="BD7" s="28"/>
+    </row>
+    <row r="8" spans="1:56">
       <c r="A8" s="14" t="s">
         <v>26</v>
       </c>
@@ -2222,21 +2241,21 @@
         <v>30</v>
       </c>
       <c r="W8" s="25"/>
-      <c r="AL8" s="5" t="s">
+      <c r="AM8" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="AS8" s="11" t="s">
+      <c r="AT8" s="11" t="s">
         <v>57</v>
       </c>
-      <c r="AW8" s="28"/>
       <c r="AX8" s="28"/>
       <c r="AY8" s="28"/>
       <c r="AZ8" s="28"/>
       <c r="BA8" s="28"/>
       <c r="BB8" s="28"/>
       <c r="BC8" s="28"/>
-    </row>
-    <row r="9" spans="1:55">
+      <c r="BD8" s="28"/>
+    </row>
+    <row r="9" spans="1:56">
       <c r="A9" s="14" t="s">
         <v>78</v>
       </c>
@@ -2281,30 +2300,30 @@
       <c r="W9" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AB9" s="35" t="s">
+      <c r="AC9" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="AC9" s="3" t="s">
+      <c r="AD9" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="AE9" s="21" t="s">
+      <c r="AF9" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="AL9" s="23" t="s">
+      <c r="AM9" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="AS9" s="11" t="s">
+      <c r="AT9" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="AW9" s="28"/>
       <c r="AX9" s="28"/>
       <c r="AY9" s="28"/>
       <c r="AZ9" s="28"/>
       <c r="BA9" s="28"/>
       <c r="BB9" s="28"/>
       <c r="BC9" s="28"/>
-    </row>
-    <row r="10" spans="1:55">
+      <c r="BD9" s="28"/>
+    </row>
+    <row r="10" spans="1:56">
       <c r="A10" s="14" t="s">
         <v>30</v>
       </c>
@@ -2349,21 +2368,21 @@
       <c r="W10" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AL10" s="5" t="s">
+      <c r="AM10" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="AS10" s="11" t="s">
+      <c r="AT10" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="AW10" s="28"/>
       <c r="AX10" s="28"/>
       <c r="AY10" s="28"/>
       <c r="AZ10" s="28"/>
       <c r="BA10" s="28"/>
       <c r="BB10" s="28"/>
       <c r="BC10" s="28"/>
-    </row>
-    <row r="11" spans="1:55">
+      <c r="BD10" s="28"/>
+    </row>
+    <row r="11" spans="1:56">
       <c r="A11" s="14" t="s">
         <v>33</v>
       </c>
@@ -2397,21 +2416,21 @@
       <c r="M11" s="15"/>
       <c r="N11" s="15"/>
       <c r="O11" s="15"/>
-      <c r="AL11" s="5" t="s">
+      <c r="AM11" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="AS11" s="11" t="s">
+      <c r="AT11" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="AW11" s="28"/>
       <c r="AX11" s="28"/>
       <c r="AY11" s="28"/>
       <c r="AZ11" s="28"/>
       <c r="BA11" s="28"/>
       <c r="BB11" s="28"/>
       <c r="BC11" s="28"/>
-    </row>
-    <row r="12" spans="1:55">
+      <c r="BD11" s="28"/>
+    </row>
+    <row r="12" spans="1:56">
       <c r="A12" s="14" t="s">
         <v>29</v>
       </c>
@@ -2451,24 +2470,24 @@
       <c r="O12" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="AB12" s="35" t="s">
+      <c r="AC12" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="AL12" s="5" t="s">
+      <c r="AM12" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="AS12" s="11" t="s">
+      <c r="AT12" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="AW12" s="28"/>
       <c r="AX12" s="28"/>
       <c r="AY12" s="28"/>
       <c r="AZ12" s="28"/>
       <c r="BA12" s="28"/>
       <c r="BB12" s="28"/>
       <c r="BC12" s="28"/>
-    </row>
-    <row r="13" spans="1:55">
+      <c r="BD12" s="28"/>
+    </row>
+    <row r="13" spans="1:56">
       <c r="A13" s="14" t="s">
         <v>79</v>
       </c>
@@ -2508,21 +2527,21 @@
       <c r="O13" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="AL13" s="5" t="s">
+      <c r="AM13" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="AS13" s="11" t="s">
+      <c r="AT13" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="AW13" s="28"/>
       <c r="AX13" s="28"/>
       <c r="AY13" s="28"/>
       <c r="AZ13" s="28"/>
       <c r="BA13" s="28"/>
       <c r="BB13" s="28"/>
       <c r="BC13" s="28"/>
-    </row>
-    <row r="14" spans="1:55" ht="12.95" customHeight="1">
+      <c r="BD13" s="28"/>
+    </row>
+    <row r="14" spans="1:56" ht="12.95" customHeight="1">
       <c r="A14" s="14" t="s">
         <v>31</v>
       </c>
@@ -2556,21 +2575,21 @@
       <c r="M14" s="15"/>
       <c r="N14" s="15"/>
       <c r="O14" s="15"/>
-      <c r="AL14" s="5" t="s">
+      <c r="AM14" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="AS14" s="11" t="s">
+      <c r="AT14" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="AW14" s="28"/>
       <c r="AX14" s="28"/>
       <c r="AY14" s="28"/>
       <c r="AZ14" s="28"/>
       <c r="BA14" s="28"/>
       <c r="BB14" s="28"/>
       <c r="BC14" s="28"/>
-    </row>
-    <row r="15" spans="1:55">
+      <c r="BD14" s="28"/>
+    </row>
+    <row r="15" spans="1:56">
       <c r="A15" s="14" t="s">
         <v>34</v>
       </c>
@@ -2604,21 +2623,21 @@
       <c r="M15" s="15"/>
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
-      <c r="AL15" s="5" t="s">
+      <c r="AM15" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="AS15" s="11" t="s">
+      <c r="AT15" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="AW15" s="28"/>
       <c r="AX15" s="28"/>
       <c r="AY15" s="28"/>
       <c r="AZ15" s="28"/>
       <c r="BA15" s="28"/>
       <c r="BB15" s="28"/>
       <c r="BC15" s="28"/>
-    </row>
-    <row r="16" spans="1:55">
+      <c r="BD15" s="28"/>
+    </row>
+    <row r="16" spans="1:56">
       <c r="A16" s="14" t="s">
         <v>32</v>
       </c>
@@ -2663,38 +2682,38 @@
       <c r="W16" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AB16" s="35" t="s">
+      <c r="AC16" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="AC16" s="3" t="s">
+      <c r="AD16" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="AE16" s="2" t="s">
+      <c r="AF16" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="AI16" s="37" t="s">
+      <c r="AJ16" s="37" t="s">
         <v>140</v>
       </c>
-      <c r="AJ16" s="22" t="s">
+      <c r="AK16" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="AK16" s="5" t="s">
+      <c r="AL16" s="5" t="s">
         <v>63</v>
       </c>
-      <c r="AL16" s="15"/>
-      <c r="AQ16" s="18"/>
-      <c r="AS16" s="9" t="s">
+      <c r="AM16" s="15"/>
+      <c r="AR16" s="18"/>
+      <c r="AT16" s="9" t="s">
         <v>125</v>
       </c>
-      <c r="AW16" s="28"/>
-      <c r="AX16" s="29"/>
-      <c r="AY16" s="28"/>
+      <c r="AX16" s="28"/>
+      <c r="AY16" s="29"/>
       <c r="AZ16" s="28"/>
       <c r="BA16" s="28"/>
       <c r="BB16" s="28"/>
       <c r="BC16" s="28"/>
-    </row>
-    <row r="17" spans="1:55">
+      <c r="BD16" s="28"/>
+    </row>
+    <row r="17" spans="1:56">
       <c r="A17" s="14" t="s">
         <v>80</v>
       </c>
@@ -2737,20 +2756,20 @@
       <c r="W17" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AJ17" s="22"/>
-      <c r="AQ17" s="18"/>
-      <c r="AS17" s="11" t="s">
+      <c r="AK17" s="22"/>
+      <c r="AR17" s="18"/>
+      <c r="AT17" s="11" t="s">
         <v>126</v>
       </c>
-      <c r="AW17" s="28"/>
-      <c r="AX17" s="29"/>
-      <c r="AY17" s="28"/>
+      <c r="AX17" s="28"/>
+      <c r="AY17" s="29"/>
       <c r="AZ17" s="28"/>
       <c r="BA17" s="28"/>
       <c r="BB17" s="28"/>
       <c r="BC17" s="28"/>
-    </row>
-    <row r="18" spans="1:55">
+      <c r="BD17" s="28"/>
+    </row>
+    <row r="18" spans="1:56">
       <c r="A18" s="14" t="s">
         <v>63</v>
       </c>
@@ -2797,28 +2816,28 @@
         <v>64</v>
       </c>
       <c r="W18" s="16"/>
-      <c r="AB18" s="35" t="s">
+      <c r="AC18" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="AC18" s="3" t="s">
+      <c r="AD18" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AE18" s="2" t="s">
+      <c r="AF18" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="AL18" s="4"/>
-      <c r="AS18" s="11" t="s">
+      <c r="AM18" s="4"/>
+      <c r="AT18" s="11" t="s">
         <v>129</v>
       </c>
-      <c r="AW18" s="28"/>
       <c r="AX18" s="28"/>
       <c r="AY18" s="28"/>
       <c r="AZ18" s="28"/>
       <c r="BA18" s="28"/>
       <c r="BB18" s="28"/>
       <c r="BC18" s="28"/>
-    </row>
-    <row r="19" spans="1:55">
+      <c r="BD18" s="28"/>
+    </row>
+    <row r="19" spans="1:56">
       <c r="A19" s="14" t="s">
         <v>81</v>
       </c>
@@ -2863,37 +2882,37 @@
       <c r="W19" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="AB19" s="35" t="s">
+      <c r="AC19" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="AC19" s="5" t="s">
+      <c r="AD19" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="AD19" s="5" t="s">
+      <c r="AE19" s="5" t="s">
         <v>64</v>
       </c>
-      <c r="AE19" s="39"/>
-      <c r="AI19" s="37" t="s">
+      <c r="AF19" s="39"/>
+      <c r="AJ19" s="37" t="s">
         <v>146</v>
       </c>
-      <c r="AJ19" s="5" t="s">
+      <c r="AK19" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="AL19" s="26" t="s">
+      <c r="AM19" s="26" t="s">
         <v>128</v>
       </c>
-      <c r="AS19" s="11" t="s">
+      <c r="AT19" s="11" t="s">
         <v>130</v>
       </c>
-      <c r="AW19" s="28"/>
       <c r="AX19" s="28"/>
       <c r="AY19" s="28"/>
       <c r="AZ19" s="28"/>
       <c r="BA19" s="28"/>
       <c r="BB19" s="28"/>
       <c r="BC19" s="28"/>
-    </row>
-    <row r="20" spans="1:55">
+      <c r="BD19" s="28"/>
+    </row>
+    <row r="20" spans="1:56">
       <c r="A20" s="19" t="s">
         <v>64</v>
       </c>
@@ -2936,16 +2955,16 @@
       <c r="W20" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="AL20" s="4"/>
-      <c r="AW20" s="28"/>
+      <c r="AM20" s="4"/>
       <c r="AX20" s="28"/>
       <c r="AY20" s="28"/>
       <c r="AZ20" s="28"/>
       <c r="BA20" s="28"/>
       <c r="BB20" s="28"/>
       <c r="BC20" s="28"/>
-    </row>
-    <row r="21" spans="1:55">
+      <c r="BD20" s="28"/>
+    </row>
+    <row r="21" spans="1:56">
       <c r="A21" s="14" t="s">
         <v>105</v>
       </c>
@@ -2973,399 +2992,399 @@
       <c r="M21" s="15" t="s">
         <v>112</v>
       </c>
-      <c r="AW21" s="28"/>
       <c r="AX21" s="28"/>
       <c r="AY21" s="28"/>
       <c r="AZ21" s="28"/>
       <c r="BA21" s="28"/>
       <c r="BB21" s="28"/>
       <c r="BC21" s="28"/>
-    </row>
-    <row r="22" spans="1:55">
+      <c r="BD21" s="28"/>
+    </row>
+    <row r="22" spans="1:56">
       <c r="M22" s="15"/>
-      <c r="AW22" s="28"/>
       <c r="AX22" s="28"/>
       <c r="AY22" s="28"/>
       <c r="AZ22" s="28"/>
       <c r="BA22" s="28"/>
       <c r="BB22" s="28"/>
       <c r="BC22" s="28"/>
-    </row>
-    <row r="23" spans="1:55">
-      <c r="AW23" s="28"/>
+      <c r="BD22" s="28"/>
+    </row>
+    <row r="23" spans="1:56">
       <c r="AX23" s="28"/>
       <c r="AY23" s="28"/>
       <c r="AZ23" s="28"/>
       <c r="BA23" s="28"/>
       <c r="BB23" s="28"/>
       <c r="BC23" s="28"/>
-    </row>
-    <row r="24" spans="1:55">
-      <c r="AW24" s="28"/>
+      <c r="BD23" s="28"/>
+    </row>
+    <row r="24" spans="1:56">
       <c r="AX24" s="28"/>
       <c r="AY24" s="28"/>
       <c r="AZ24" s="28"/>
       <c r="BA24" s="28"/>
       <c r="BB24" s="28"/>
       <c r="BC24" s="28"/>
-    </row>
-    <row r="25" spans="1:55">
-      <c r="AW25" s="28"/>
+      <c r="BD24" s="28"/>
+    </row>
+    <row r="25" spans="1:56">
       <c r="AX25" s="28"/>
       <c r="AY25" s="28"/>
       <c r="AZ25" s="28"/>
       <c r="BA25" s="28"/>
       <c r="BB25" s="28"/>
       <c r="BC25" s="28"/>
-    </row>
-    <row r="26" spans="1:55">
-      <c r="AW26" s="28"/>
+      <c r="BD25" s="28"/>
+    </row>
+    <row r="26" spans="1:56">
       <c r="AX26" s="28"/>
       <c r="AY26" s="28"/>
       <c r="AZ26" s="28"/>
       <c r="BA26" s="28"/>
       <c r="BB26" s="28"/>
       <c r="BC26" s="28"/>
-    </row>
-    <row r="27" spans="1:55">
-      <c r="AW27" s="28"/>
+      <c r="BD26" s="28"/>
+    </row>
+    <row r="27" spans="1:56">
       <c r="AX27" s="28"/>
       <c r="AY27" s="28"/>
       <c r="AZ27" s="28"/>
       <c r="BA27" s="28"/>
       <c r="BB27" s="28"/>
       <c r="BC27" s="28"/>
-    </row>
-    <row r="28" spans="1:55">
-      <c r="AW28" s="28"/>
+      <c r="BD27" s="28"/>
+    </row>
+    <row r="28" spans="1:56">
       <c r="AX28" s="28"/>
       <c r="AY28" s="28"/>
       <c r="AZ28" s="28"/>
       <c r="BA28" s="28"/>
       <c r="BB28" s="28"/>
       <c r="BC28" s="28"/>
-    </row>
-    <row r="29" spans="1:55">
-      <c r="AW29" s="28"/>
+      <c r="BD28" s="28"/>
+    </row>
+    <row r="29" spans="1:56">
       <c r="AX29" s="28"/>
       <c r="AY29" s="28"/>
       <c r="AZ29" s="28"/>
       <c r="BA29" s="28"/>
       <c r="BB29" s="28"/>
       <c r="BC29" s="28"/>
-    </row>
-    <row r="30" spans="1:55">
-      <c r="AW30" s="28"/>
+      <c r="BD29" s="28"/>
+    </row>
+    <row r="30" spans="1:56">
       <c r="AX30" s="28"/>
       <c r="AY30" s="28"/>
       <c r="AZ30" s="28"/>
       <c r="BA30" s="28"/>
       <c r="BB30" s="28"/>
       <c r="BC30" s="28"/>
-    </row>
-    <row r="31" spans="1:55">
-      <c r="AW31" s="28"/>
+      <c r="BD30" s="28"/>
+    </row>
+    <row r="31" spans="1:56">
       <c r="AX31" s="28"/>
       <c r="AY31" s="28"/>
       <c r="AZ31" s="28"/>
       <c r="BA31" s="28"/>
       <c r="BB31" s="28"/>
       <c r="BC31" s="28"/>
-    </row>
-    <row r="32" spans="1:55">
-      <c r="AW32" s="28"/>
+      <c r="BD31" s="28"/>
+    </row>
+    <row r="32" spans="1:56">
       <c r="AX32" s="28"/>
       <c r="AY32" s="28"/>
       <c r="AZ32" s="28"/>
       <c r="BA32" s="28"/>
       <c r="BB32" s="28"/>
       <c r="BC32" s="28"/>
-    </row>
-    <row r="33" spans="49:55">
-      <c r="AW33" s="24"/>
+      <c r="BD32" s="28"/>
+    </row>
+    <row r="33" spans="50:56">
       <c r="AX33" s="24"/>
       <c r="AY33" s="24"/>
       <c r="AZ33" s="24"/>
       <c r="BA33" s="24"/>
       <c r="BB33" s="24"/>
       <c r="BC33" s="24"/>
-    </row>
-    <row r="34" spans="49:55">
-      <c r="AW34" s="24"/>
+      <c r="BD33" s="24"/>
+    </row>
+    <row r="34" spans="50:56">
       <c r="AX34" s="24"/>
       <c r="AY34" s="24"/>
       <c r="AZ34" s="24"/>
       <c r="BA34" s="24"/>
       <c r="BB34" s="24"/>
       <c r="BC34" s="24"/>
-    </row>
-    <row r="35" spans="49:55">
-      <c r="AW35" s="24"/>
+      <c r="BD34" s="24"/>
+    </row>
+    <row r="35" spans="50:56">
       <c r="AX35" s="24"/>
       <c r="AY35" s="24"/>
       <c r="AZ35" s="24"/>
       <c r="BA35" s="24"/>
       <c r="BB35" s="24"/>
       <c r="BC35" s="24"/>
-    </row>
-    <row r="36" spans="49:55">
-      <c r="AW36" s="24"/>
+      <c r="BD35" s="24"/>
+    </row>
+    <row r="36" spans="50:56">
       <c r="AX36" s="24"/>
       <c r="AY36" s="24"/>
       <c r="AZ36" s="24"/>
       <c r="BA36" s="24"/>
       <c r="BB36" s="24"/>
       <c r="BC36" s="24"/>
-    </row>
-    <row r="37" spans="49:55">
-      <c r="AW37" s="24"/>
+      <c r="BD36" s="24"/>
+    </row>
+    <row r="37" spans="50:56">
       <c r="AX37" s="24"/>
       <c r="AY37" s="24"/>
       <c r="AZ37" s="24"/>
       <c r="BA37" s="24"/>
       <c r="BB37" s="24"/>
       <c r="BC37" s="24"/>
-    </row>
-    <row r="38" spans="49:55">
-      <c r="AW38" s="24"/>
+      <c r="BD37" s="24"/>
+    </row>
+    <row r="38" spans="50:56">
       <c r="AX38" s="24"/>
       <c r="AY38" s="24"/>
       <c r="AZ38" s="24"/>
       <c r="BA38" s="24"/>
       <c r="BB38" s="24"/>
       <c r="BC38" s="24"/>
-    </row>
-    <row r="39" spans="49:55">
-      <c r="AW39" s="24"/>
+      <c r="BD38" s="24"/>
+    </row>
+    <row r="39" spans="50:56">
       <c r="AX39" s="24"/>
       <c r="AY39" s="24"/>
       <c r="AZ39" s="24"/>
       <c r="BA39" s="24"/>
       <c r="BB39" s="24"/>
       <c r="BC39" s="24"/>
-    </row>
-    <row r="40" spans="49:55">
-      <c r="AW40" s="24"/>
+      <c r="BD39" s="24"/>
+    </row>
+    <row r="40" spans="50:56">
       <c r="AX40" s="24"/>
       <c r="AY40" s="24"/>
       <c r="AZ40" s="24"/>
       <c r="BA40" s="24"/>
       <c r="BB40" s="24"/>
       <c r="BC40" s="24"/>
-    </row>
-    <row r="41" spans="49:55">
-      <c r="AW41" s="24"/>
+      <c r="BD40" s="24"/>
+    </row>
+    <row r="41" spans="50:56">
       <c r="AX41" s="24"/>
       <c r="AY41" s="24"/>
       <c r="AZ41" s="24"/>
       <c r="BA41" s="24"/>
       <c r="BB41" s="24"/>
       <c r="BC41" s="24"/>
-    </row>
-    <row r="42" spans="49:55">
-      <c r="AW42" s="24"/>
+      <c r="BD41" s="24"/>
+    </row>
+    <row r="42" spans="50:56">
       <c r="AX42" s="24"/>
       <c r="AY42" s="24"/>
       <c r="AZ42" s="24"/>
       <c r="BA42" s="24"/>
       <c r="BB42" s="24"/>
       <c r="BC42" s="24"/>
-    </row>
-    <row r="43" spans="49:55">
-      <c r="AW43" s="24"/>
+      <c r="BD42" s="24"/>
+    </row>
+    <row r="43" spans="50:56">
       <c r="AX43" s="24"/>
       <c r="AY43" s="24"/>
       <c r="AZ43" s="24"/>
       <c r="BA43" s="24"/>
       <c r="BB43" s="24"/>
       <c r="BC43" s="24"/>
-    </row>
-    <row r="44" spans="49:55">
-      <c r="AW44" s="24"/>
+      <c r="BD43" s="24"/>
+    </row>
+    <row r="44" spans="50:56">
       <c r="AX44" s="24"/>
       <c r="AY44" s="24"/>
       <c r="AZ44" s="24"/>
       <c r="BA44" s="24"/>
       <c r="BB44" s="24"/>
       <c r="BC44" s="24"/>
-    </row>
-    <row r="45" spans="49:55">
-      <c r="AW45" s="24"/>
+      <c r="BD44" s="24"/>
+    </row>
+    <row r="45" spans="50:56">
       <c r="AX45" s="24"/>
       <c r="AY45" s="24"/>
       <c r="AZ45" s="24"/>
       <c r="BA45" s="24"/>
       <c r="BB45" s="24"/>
       <c r="BC45" s="24"/>
-    </row>
-    <row r="46" spans="49:55">
-      <c r="AW46" s="24"/>
+      <c r="BD45" s="24"/>
+    </row>
+    <row r="46" spans="50:56">
       <c r="AX46" s="24"/>
       <c r="AY46" s="24"/>
       <c r="AZ46" s="24"/>
       <c r="BA46" s="24"/>
       <c r="BB46" s="24"/>
       <c r="BC46" s="24"/>
-    </row>
-    <row r="47" spans="49:55">
-      <c r="AW47" s="24"/>
+      <c r="BD46" s="24"/>
+    </row>
+    <row r="47" spans="50:56">
       <c r="AX47" s="24"/>
       <c r="AY47" s="24"/>
       <c r="AZ47" s="24"/>
       <c r="BA47" s="24"/>
       <c r="BB47" s="24"/>
       <c r="BC47" s="24"/>
-    </row>
-    <row r="48" spans="49:55">
-      <c r="AW48" s="24"/>
+      <c r="BD47" s="24"/>
+    </row>
+    <row r="48" spans="50:56">
       <c r="AX48" s="24"/>
       <c r="AY48" s="24"/>
       <c r="AZ48" s="24"/>
       <c r="BA48" s="24"/>
       <c r="BB48" s="24"/>
       <c r="BC48" s="24"/>
-    </row>
-    <row r="49" spans="49:55">
-      <c r="AW49" s="24"/>
+      <c r="BD48" s="24"/>
+    </row>
+    <row r="49" spans="50:56">
       <c r="AX49" s="24"/>
       <c r="AY49" s="24"/>
       <c r="AZ49" s="24"/>
       <c r="BA49" s="24"/>
       <c r="BB49" s="24"/>
       <c r="BC49" s="24"/>
-    </row>
-    <row r="50" spans="49:55">
-      <c r="AW50" s="24"/>
+      <c r="BD49" s="24"/>
+    </row>
+    <row r="50" spans="50:56">
       <c r="AX50" s="24"/>
       <c r="AY50" s="24"/>
       <c r="AZ50" s="24"/>
       <c r="BA50" s="24"/>
       <c r="BB50" s="24"/>
       <c r="BC50" s="24"/>
-    </row>
-    <row r="51" spans="49:55">
-      <c r="AW51" s="24"/>
+      <c r="BD50" s="24"/>
+    </row>
+    <row r="51" spans="50:56">
       <c r="AX51" s="24"/>
       <c r="AY51" s="24"/>
       <c r="AZ51" s="24"/>
       <c r="BA51" s="24"/>
       <c r="BB51" s="24"/>
       <c r="BC51" s="24"/>
-    </row>
-    <row r="52" spans="49:55">
-      <c r="AW52" s="24"/>
+      <c r="BD51" s="24"/>
+    </row>
+    <row r="52" spans="50:56">
       <c r="AX52" s="24"/>
       <c r="AY52" s="24"/>
       <c r="AZ52" s="24"/>
       <c r="BA52" s="24"/>
       <c r="BB52" s="24"/>
       <c r="BC52" s="24"/>
-    </row>
-    <row r="53" spans="49:55">
-      <c r="AW53" s="24"/>
+      <c r="BD52" s="24"/>
+    </row>
+    <row r="53" spans="50:56">
       <c r="AX53" s="24"/>
       <c r="AY53" s="24"/>
       <c r="AZ53" s="24"/>
       <c r="BA53" s="24"/>
       <c r="BB53" s="24"/>
       <c r="BC53" s="24"/>
-    </row>
-    <row r="54" spans="49:55">
-      <c r="AW54" s="24"/>
+      <c r="BD53" s="24"/>
+    </row>
+    <row r="54" spans="50:56">
       <c r="AX54" s="24"/>
       <c r="AY54" s="24"/>
       <c r="AZ54" s="24"/>
       <c r="BA54" s="24"/>
       <c r="BB54" s="24"/>
       <c r="BC54" s="24"/>
-    </row>
-    <row r="55" spans="49:55">
-      <c r="AW55" s="24"/>
+      <c r="BD54" s="24"/>
+    </row>
+    <row r="55" spans="50:56">
       <c r="AX55" s="24"/>
       <c r="AY55" s="24"/>
       <c r="AZ55" s="24"/>
       <c r="BA55" s="24"/>
       <c r="BB55" s="24"/>
       <c r="BC55" s="24"/>
-    </row>
-    <row r="56" spans="49:55">
-      <c r="AW56" s="24"/>
+      <c r="BD55" s="24"/>
+    </row>
+    <row r="56" spans="50:56">
       <c r="AX56" s="24"/>
       <c r="AY56" s="24"/>
       <c r="AZ56" s="24"/>
       <c r="BA56" s="24"/>
       <c r="BB56" s="24"/>
       <c r="BC56" s="24"/>
-    </row>
-    <row r="57" spans="49:55">
-      <c r="AW57" s="24"/>
+      <c r="BD56" s="24"/>
+    </row>
+    <row r="57" spans="50:56">
       <c r="AX57" s="24"/>
       <c r="AY57" s="24"/>
       <c r="AZ57" s="24"/>
       <c r="BA57" s="24"/>
       <c r="BB57" s="24"/>
       <c r="BC57" s="24"/>
-    </row>
-    <row r="58" spans="49:55">
-      <c r="AW58" s="24"/>
+      <c r="BD57" s="24"/>
+    </row>
+    <row r="58" spans="50:56">
       <c r="AX58" s="24"/>
       <c r="AY58" s="24"/>
       <c r="AZ58" s="24"/>
       <c r="BA58" s="24"/>
       <c r="BB58" s="24"/>
       <c r="BC58" s="24"/>
-    </row>
-    <row r="59" spans="49:55">
-      <c r="AW59" s="24"/>
+      <c r="BD58" s="24"/>
+    </row>
+    <row r="59" spans="50:56">
       <c r="AX59" s="24"/>
       <c r="AY59" s="24"/>
       <c r="AZ59" s="24"/>
       <c r="BA59" s="24"/>
       <c r="BB59" s="24"/>
       <c r="BC59" s="24"/>
-    </row>
-    <row r="60" spans="49:55">
-      <c r="BB60" s="11"/>
+      <c r="BD59" s="24"/>
+    </row>
+    <row r="60" spans="50:56">
       <c r="BC60" s="11"/>
-    </row>
-    <row r="61" spans="49:55">
-      <c r="BB61" s="11"/>
+      <c r="BD60" s="11"/>
+    </row>
+    <row r="61" spans="50:56">
       <c r="BC61" s="11"/>
-    </row>
-    <row r="62" spans="49:55">
-      <c r="BB62" s="11"/>
+      <c r="BD61" s="11"/>
+    </row>
+    <row r="62" spans="50:56">
       <c r="BC62" s="11"/>
-    </row>
-    <row r="63" spans="49:55">
-      <c r="BB63" s="11"/>
+      <c r="BD62" s="11"/>
+    </row>
+    <row r="63" spans="50:56">
       <c r="BC63" s="11"/>
-    </row>
-    <row r="64" spans="49:55">
-      <c r="BB64" s="11"/>
+      <c r="BD63" s="11"/>
+    </row>
+    <row r="64" spans="50:56">
       <c r="BC64" s="11"/>
-    </row>
-    <row r="65" spans="54:55">
-      <c r="BB65" s="11"/>
+      <c r="BD64" s="11"/>
+    </row>
+    <row r="65" spans="55:56">
       <c r="BC65" s="11"/>
-    </row>
-    <row r="66" spans="54:55">
-      <c r="BB66" s="11"/>
+      <c r="BD65" s="11"/>
+    </row>
+    <row r="66" spans="55:56">
       <c r="BC66" s="11"/>
-    </row>
-    <row r="67" spans="54:55">
-      <c r="BB67" s="11"/>
+      <c r="BD66" s="11"/>
+    </row>
+    <row r="67" spans="55:56">
       <c r="BC67" s="11"/>
-    </row>
-    <row r="68" spans="54:55">
-      <c r="BB68" s="11"/>
+      <c r="BD67" s="11"/>
+    </row>
+    <row r="68" spans="55:56">
       <c r="BC68" s="11"/>
+      <c r="BD68" s="11"/>
     </row>
   </sheetData>
-  <sortState ref="AD5:AF6">
-    <sortCondition descending="1" ref="AF5"/>
+  <sortState ref="AE5:AG6">
+    <sortCondition descending="1" ref="AG5"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
make experience handle up to 5 codes in spreadsheet
</commit_message>
<xml_diff>
--- a/scoretools/test/mkGameEngine2.xlsx
+++ b/scoretools/test/mkGameEngine2.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="379" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="153">
   <si>
     <t>stage</t>
   </si>
@@ -482,10 +482,10 @@
     <t>app</t>
   </si>
   <si>
-    <t>success</t>
-  </si>
-  <si>
-    <t>test:123</t>
+    <t>success:4:true</t>
+  </si>
+  <si>
+    <t>test:1:false</t>
   </si>
 </sst>
 </file>
@@ -1565,8 +1565,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BD68"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AB4" sqref="AB4"/>
+    <sheetView tabSelected="1" topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AU2" sqref="AU2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -1871,6 +1871,9 @@
       <c r="AP2" s="5">
         <v>1</v>
       </c>
+      <c r="AR2" s="11" t="s">
+        <v>74</v>
+      </c>
       <c r="AT2" s="11" t="s">
         <v>52</v>
       </c>

</xml_diff>